<commit_message>
Fixed typo in Self-Billing
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Document types v9.1.xlsx
+++ b/work-in-progress/Peppol Code Lists - Document types v9.1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\edec-codelists\work-in-progress\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\peppol-edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B67DC98C-2C40-47DF-B048-8DC54ABFA92F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3370B237-0139-49FC-AE9C-37E4C23F9A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Document Type" sheetId="5" r:id="rId1"/>
@@ -2300,12 +2300,6 @@
     <t>Digital Post</t>
   </si>
   <si>
-    <t>Peppol BIS SelfBilling UBL Invoice V3</t>
-  </si>
-  <si>
-    <t>Peppol BIS SelfBilling UBL CreditNote V3</t>
-  </si>
-  <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:Invoice-2::Invoice##urn:cen.eu:en16931:2017#compliant#urn:fdc:peppol.eu:2017:poacc:selfbilling:3.0::2.1</t>
   </si>
   <si>
@@ -2396,6 +2390,12 @@
     <t>cenbii-procid-ubl::urn:fdc:peppol.eu:poacc:bis:invoice_response:3
 cenbii-procid-ubl::urn:peppol:france:billing:regulated
 cenbii-procid-ubl::urn:peppol:france:billing:non-regulated</t>
+  </si>
+  <si>
+    <t>Peppol BIS Self-Billing UBL Invoice V3</t>
+  </si>
+  <si>
+    <t>Peppol BIS Self-Billing UBL CreditNote V3</t>
   </si>
 </sst>
 </file>
@@ -3058,9 +3058,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45987FB-91F4-488D-A9D3-2F3FAED3E07C}">
   <dimension ref="A1:N277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N55" sqref="N55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4340,7 +4340,7 @@
         <v>366</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="I32" s="5" t="b">
         <v>0</v>
@@ -4359,7 +4359,7 @@
         <v>718</v>
       </c>
       <c r="N32" s="5" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -4379,7 +4379,7 @@
         <v>366</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="I33" s="5" t="b">
         <v>0</v>
@@ -4398,7 +4398,7 @@
         <v>719</v>
       </c>
       <c r="N33" s="5" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -5246,7 +5246,7 @@
         <v>366</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="I55" s="5" t="b">
         <v>0</v>
@@ -5265,7 +5265,7 @@
         <v>725</v>
       </c>
       <c r="N55" s="5" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
     </row>
     <row r="56" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -13197,22 +13197,22 @@
     </row>
     <row r="269" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A269" s="5" t="s">
+        <v>762</v>
+      </c>
+      <c r="B269" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C269" s="5" t="s">
         <v>734</v>
       </c>
-      <c r="B269" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C269" s="5" t="s">
+      <c r="D269" s="27" t="s">
         <v>736</v>
       </c>
-      <c r="D269" s="27" t="s">
-        <v>738</v>
-      </c>
       <c r="E269" s="23" t="s">
         <v>366</v>
       </c>
       <c r="H269" s="5" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="I269" s="5" t="b">
         <v>0</v>
@@ -13231,27 +13231,27 @@
         <v>718</v>
       </c>
       <c r="N269" s="5" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
     </row>
     <row r="270" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A270" s="5" t="s">
+        <v>763</v>
+      </c>
+      <c r="B270" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C270" s="5" t="s">
         <v>735</v>
       </c>
-      <c r="B270" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C270" s="5" t="s">
-        <v>737</v>
-      </c>
       <c r="D270" s="27" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="E270" s="23" t="s">
         <v>366</v>
       </c>
       <c r="H270" s="5" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="I270" s="5" t="b">
         <v>0</v>
@@ -13270,27 +13270,27 @@
         <v>719</v>
       </c>
       <c r="N270" s="5" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
     </row>
     <row r="271" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A271" s="5" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="B271" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C271" s="5" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="D271" s="27" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="E271" s="23" t="s">
         <v>366</v>
       </c>
       <c r="H271" s="5" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="I271" s="5" t="b">
         <v>0</v>
@@ -13302,30 +13302,30 @@
         <v>601</v>
       </c>
       <c r="M271" s="23" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="N271" s="5" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
     </row>
     <row r="272" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A272" s="5" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="B272" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C272" s="5" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="D272" s="27" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="E272" s="23" t="s">
         <v>366</v>
       </c>
       <c r="H272" s="5" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="I272" s="5" t="b">
         <v>0</v>
@@ -13338,33 +13338,33 @@
         <v>1</v>
       </c>
       <c r="L272" s="23" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="M272" s="23" t="s">
         <v>718</v>
       </c>
       <c r="N272" s="5" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
     </row>
     <row r="273" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A273" s="5" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="B273" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C273" s="5" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="D273" s="27" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="E273" s="23" t="s">
         <v>366</v>
       </c>
       <c r="H273" s="5" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="I273" s="5" t="b">
         <v>0</v>
@@ -13377,33 +13377,33 @@
         <v>1</v>
       </c>
       <c r="L273" s="23" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="M273" s="23" t="s">
         <v>718</v>
       </c>
       <c r="N273" s="5" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
     </row>
     <row r="274" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A274" s="5" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="B274" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C274" s="5" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="D274" s="27" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="E274" s="23" t="s">
         <v>366</v>
       </c>
       <c r="H274" s="5" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="I274" s="5" t="b">
         <v>0</v>
@@ -13416,33 +13416,33 @@
         <v>1</v>
       </c>
       <c r="L274" s="23" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="M274" s="23" t="s">
         <v>718</v>
       </c>
       <c r="N274" s="5" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
     </row>
     <row r="275" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A275" s="5" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="B275" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C275" s="5" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="D275" s="27" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="E275" s="23" t="s">
         <v>366</v>
       </c>
       <c r="H275" s="5" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="I275" s="5" t="b">
         <v>0</v>
@@ -13455,33 +13455,33 @@
         <v>1</v>
       </c>
       <c r="L275" s="23" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="M275" s="23" t="s">
         <v>718</v>
       </c>
       <c r="N275" s="5" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
     </row>
     <row r="276" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A276" s="5" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="B276" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C276" s="5" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="D276" s="27" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="E276" s="23" t="s">
         <v>366</v>
       </c>
       <c r="H276" s="5" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="I276" s="5" t="b">
         <v>0</v>
@@ -13494,33 +13494,33 @@
         <v>1</v>
       </c>
       <c r="L276" s="23" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="M276" s="23" t="s">
         <v>718</v>
       </c>
       <c r="N276" s="5" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
     </row>
     <row r="277" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A277" s="5" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="B277" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C277" s="5" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="D277" s="27" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="E277" s="23" t="s">
         <v>366</v>
       </c>
       <c r="H277" s="5" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="I277" s="5" t="b">
         <v>0</v>
@@ -13533,13 +13533,13 @@
         <v>1</v>
       </c>
       <c r="L277" s="23" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="M277" s="23" t="s">
         <v>725</v>
       </c>
       <c r="N277" s="5" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added France UBL CreditNote doc types; TICC-371
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Document types v9.1.xlsx
+++ b/work-in-progress/Peppol Code Lists - Document types v9.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\peppol-edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3370B237-0139-49FC-AE9C-37E4C23F9A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA29540-531F-43DA-813B-4124C991B68E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25665" yWindow="0" windowWidth="26040" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Document Type" sheetId="5" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2424" uniqueCount="764">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2442" uniqueCount="770">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -2396,6 +2396,24 @@
   </si>
   <si>
     <t>Peppol BIS Self-Billing UBL CreditNote V3</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:CreditNote-2::CreditNote##urn:cen.eu:en16931:2017#compliant#urn:peppol:france:billing:cius:1.0::2.1</t>
+  </si>
+  <si>
+    <t>France UBL CreditNote CIUS</t>
+  </si>
+  <si>
+    <t>France UBL CreditNote Extension</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:CreditNote-2::CreditNote##urn:cen.eu:en16931:2017#conformant#urn:peppol:france:billing:extended:1.0::2.1</t>
+  </si>
+  <si>
+    <t>9.1</t>
+  </si>
+  <si>
+    <t>TICC-371</t>
   </si>
 </sst>
 </file>
@@ -3056,11 +3074,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45987FB-91F4-488D-A9D3-2F3FAED3E07C}">
-  <dimension ref="A1:N277"/>
+  <dimension ref="A1:N279"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C74" sqref="C74"/>
+      <pane ySplit="1" topLeftCell="A260" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A279" sqref="A279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13542,6 +13560,84 @@
         <v>743</v>
       </c>
     </row>
+    <row r="278" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A278" s="5" t="s">
+        <v>765</v>
+      </c>
+      <c r="B278" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C278" s="5" t="s">
+        <v>764</v>
+      </c>
+      <c r="D278" s="28" t="s">
+        <v>768</v>
+      </c>
+      <c r="E278" s="23" t="s">
+        <v>366</v>
+      </c>
+      <c r="H278" s="5" t="s">
+        <v>769</v>
+      </c>
+      <c r="I278" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J278" s="5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="K278" s="23">
+        <v>1</v>
+      </c>
+      <c r="L278" s="23" t="s">
+        <v>744</v>
+      </c>
+      <c r="M278" s="23" t="s">
+        <v>718</v>
+      </c>
+      <c r="N278" s="5" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="279" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A279" s="5" t="s">
+        <v>766</v>
+      </c>
+      <c r="B279" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C279" s="5" t="s">
+        <v>767</v>
+      </c>
+      <c r="D279" s="28" t="s">
+        <v>768</v>
+      </c>
+      <c r="E279" s="23" t="s">
+        <v>366</v>
+      </c>
+      <c r="H279" s="5" t="s">
+        <v>769</v>
+      </c>
+      <c r="I279" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J279" s="5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="K279" s="23">
+        <v>1</v>
+      </c>
+      <c r="L279" s="23" t="s">
+        <v>744</v>
+      </c>
+      <c r="M279" s="23" t="s">
+        <v>718</v>
+      </c>
+      <c r="N279" s="5" t="s">
+        <v>743</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:N268" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added AE PINT DocTypes; TICC-373; Fixed French CN Categories
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Document types v9.1.xlsx
+++ b/work-in-progress/Peppol Code Lists - Document types v9.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\peppol-edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA29540-531F-43DA-813B-4124C991B68E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C9139B6-A8F2-4346-972A-2473F6BF92C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25665" yWindow="0" windowWidth="26040" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="23730" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Document Type" sheetId="5" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2442" uniqueCount="770">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2478" uniqueCount="779">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -2414,6 +2414,33 @@
   </si>
   <si>
     <t>TICC-371</t>
+  </si>
+  <si>
+    <t>AE PINT Invoice v1.0</t>
+  </si>
+  <si>
+    <t>AE PINT Credit Note v1.0</t>
+  </si>
+  <si>
+    <t>AE PINT Self-Billing Invoice v1.0</t>
+  </si>
+  <si>
+    <t>AE PINT Self-Billing Credit Note v1.0</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:Invoice-2::Invoice##urn:peppol:pint:billing-1@ae-1::2.1</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:CreditNote-2::CreditNote##urn:peppol:pint:billing-1@ae-1::2.1</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:Invoice-2::Invoice##urn:peppol:pint:selfbilling-1@ae-1::2.1</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:CreditNote-2::CreditNote##urn:peppol:pint:selfbilling-1@ae-1::2.1</t>
+  </si>
+  <si>
+    <t>TICC-373</t>
   </si>
 </sst>
 </file>
@@ -3074,11 +3101,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45987FB-91F4-488D-A9D3-2F3FAED3E07C}">
-  <dimension ref="A1:N279"/>
+  <dimension ref="A1:N283"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A260" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A279" sqref="A279"/>
+      <pane ySplit="1" topLeftCell="A269" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A283" sqref="A283"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13593,7 +13620,7 @@
         <v>744</v>
       </c>
       <c r="M278" s="23" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="N278" s="5" t="s">
         <v>743</v>
@@ -13632,10 +13659,166 @@
         <v>744</v>
       </c>
       <c r="M279" s="23" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="N279" s="5" t="s">
         <v>743</v>
+      </c>
+    </row>
+    <row r="280" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>770</v>
+      </c>
+      <c r="B280" s="5" t="s">
+        <v>609</v>
+      </c>
+      <c r="C280" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="D280" s="28" t="s">
+        <v>768</v>
+      </c>
+      <c r="E280" s="23" t="s">
+        <v>366</v>
+      </c>
+      <c r="H280" s="5" t="s">
+        <v>778</v>
+      </c>
+      <c r="I280" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J280" s="5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="K280" s="23">
+        <v>3</v>
+      </c>
+      <c r="L280" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="M280" s="23" t="s">
+        <v>718</v>
+      </c>
+      <c r="N280" s="5" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="281" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>771</v>
+      </c>
+      <c r="B281" s="5" t="s">
+        <v>609</v>
+      </c>
+      <c r="C281" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="D281" s="28" t="s">
+        <v>768</v>
+      </c>
+      <c r="E281" s="23" t="s">
+        <v>366</v>
+      </c>
+      <c r="H281" s="5" t="s">
+        <v>778</v>
+      </c>
+      <c r="I281" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J281" s="5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="K281" s="23">
+        <v>3</v>
+      </c>
+      <c r="L281" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="M281" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N281" s="5" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="282" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>772</v>
+      </c>
+      <c r="B282" s="5" t="s">
+        <v>609</v>
+      </c>
+      <c r="C282" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="D282" s="28" t="s">
+        <v>768</v>
+      </c>
+      <c r="E282" s="23" t="s">
+        <v>366</v>
+      </c>
+      <c r="H282" s="5" t="s">
+        <v>778</v>
+      </c>
+      <c r="I282" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J282" s="5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="K282" s="23">
+        <v>3</v>
+      </c>
+      <c r="L282" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="M282" s="23" t="s">
+        <v>718</v>
+      </c>
+      <c r="N282" s="5" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="283" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>773</v>
+      </c>
+      <c r="B283" s="5" t="s">
+        <v>609</v>
+      </c>
+      <c r="C283" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="D283" s="28" t="s">
+        <v>768</v>
+      </c>
+      <c r="E283" s="23" t="s">
+        <v>366</v>
+      </c>
+      <c r="H283" s="5" t="s">
+        <v>778</v>
+      </c>
+      <c r="I283" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J283" s="5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="K283" s="23">
+        <v>3</v>
+      </c>
+      <c r="L283" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="M283" s="23" t="s">
+        <v>719</v>
+      </c>
+      <c r="N283" s="5" t="s">
+        <v>528</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deprecated MY PINT DocTypes with busdox-docid-qns; TICC-374
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Document types v9.1.xlsx
+++ b/work-in-progress/Peppol Code Lists - Document types v9.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\peppol-edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05DA6A8F-7EF7-46C0-A70C-367E5877E6BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC42692-FB72-4D61-94CD-3C1D06F73239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2015,9 +2015,6 @@
     <t>TICC-312</t>
   </si>
   <si>
-    <t>TICC-328</t>
-  </si>
-  <si>
     <t>Abstract?</t>
   </si>
   <si>
@@ -2449,6 +2446,10 @@
   </si>
   <si>
     <t>deprecation-scheduled</t>
+  </si>
+  <si>
+    <t>TICC-328
+TICC-374</t>
   </si>
 </sst>
 </file>
@@ -2578,7 +2579,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2713,6 +2714,16 @@
     </xf>
     <xf numFmtId="14" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3130,8 +3141,8 @@
   <dimension ref="A1:N283"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A217" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E230" sqref="E230"/>
+      <pane ySplit="1" topLeftCell="A262" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A283" sqref="A283"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3170,7 +3181,7 @@
         <v>350</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="G1" s="12" t="s">
         <v>400</v>
@@ -3179,7 +3190,7 @@
         <v>107</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>431</v>
@@ -3191,7 +3202,7 @@
         <v>109</v>
       </c>
       <c r="M1" s="22" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>152</v>
@@ -3231,7 +3242,7 @@
         <v>110</v>
       </c>
       <c r="M2" s="33" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N2" s="36" t="s">
         <v>138</v>
@@ -3271,7 +3282,7 @@
         <v>110</v>
       </c>
       <c r="M3" s="33" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N3" s="36" t="s">
         <v>138</v>
@@ -3311,7 +3322,7 @@
         <v>110</v>
       </c>
       <c r="M4" s="33" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N4" s="36" t="s">
         <v>138</v>
@@ -3351,7 +3362,7 @@
         <v>111</v>
       </c>
       <c r="M5" s="33" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="N5" s="36" t="s">
         <v>139</v>
@@ -3391,7 +3402,7 @@
         <v>111</v>
       </c>
       <c r="M6" s="33" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="N6" s="36" t="s">
         <v>140</v>
@@ -3431,7 +3442,7 @@
         <v>111</v>
       </c>
       <c r="M7" s="33" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="N7" s="36" t="s">
         <v>139</v>
@@ -3471,7 +3482,7 @@
         <v>111</v>
       </c>
       <c r="M8" s="33" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="N8" s="36" t="s">
         <v>141</v>
@@ -3511,7 +3522,7 @@
         <v>111</v>
       </c>
       <c r="M9" s="33" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="N9" s="36" t="s">
         <v>142</v>
@@ -3554,7 +3565,7 @@
         <v>111</v>
       </c>
       <c r="M10" s="33" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="N10" s="36" t="s">
         <v>143</v>
@@ -3594,7 +3605,7 @@
         <v>111</v>
       </c>
       <c r="M11" s="33" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="N11" s="36" t="s">
         <v>143</v>
@@ -3634,7 +3645,7 @@
         <v>111</v>
       </c>
       <c r="M12" s="33" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N12" s="36" t="s">
         <v>144</v>
@@ -3674,7 +3685,7 @@
         <v>111</v>
       </c>
       <c r="M13" s="33" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N13" s="36" t="s">
         <v>145</v>
@@ -3714,7 +3725,7 @@
         <v>111</v>
       </c>
       <c r="M14" s="33" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N14" s="36" t="s">
         <v>146</v>
@@ -3722,7 +3733,7 @@
     </row>
     <row r="15" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B15" s="31" t="s">
         <v>56</v>
@@ -3754,7 +3765,7 @@
         <v>111</v>
       </c>
       <c r="M15" s="33" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N15" s="36" t="s">
         <v>146</v>
@@ -3794,7 +3805,7 @@
         <v>111</v>
       </c>
       <c r="M16" s="33" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N16" s="36" t="s">
         <v>146</v>
@@ -3834,7 +3845,7 @@
         <v>111</v>
       </c>
       <c r="M17" s="33" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N17" s="36" t="s">
         <v>147</v>
@@ -3842,7 +3853,7 @@
     </row>
     <row r="18" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="B18" s="31" t="s">
         <v>56</v>
@@ -3874,7 +3885,7 @@
         <v>111</v>
       </c>
       <c r="M18" s="33" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N18" s="36" t="s">
         <v>147</v>
@@ -3914,7 +3925,7 @@
         <v>111</v>
       </c>
       <c r="M19" s="33" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="N19" s="36" t="s">
         <v>148</v>
@@ -3954,7 +3965,7 @@
         <v>111</v>
       </c>
       <c r="M20" s="33" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="N20" s="36" t="s">
         <v>148</v>
@@ -3994,7 +4005,7 @@
         <v>111</v>
       </c>
       <c r="M21" s="33" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="N21" s="36" t="s">
         <v>148</v>
@@ -4034,7 +4045,7 @@
         <v>111</v>
       </c>
       <c r="M22" s="33" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N22" s="36" t="s">
         <v>148</v>
@@ -4042,7 +4053,7 @@
     </row>
     <row r="23" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="36" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="B23" s="31" t="s">
         <v>56</v>
@@ -4074,7 +4085,7 @@
         <v>111</v>
       </c>
       <c r="M23" s="33" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N23" s="36" t="s">
         <v>148</v>
@@ -4114,7 +4125,7 @@
         <v>111</v>
       </c>
       <c r="M24" s="33" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N24" s="36" t="s">
         <v>148</v>
@@ -4152,7 +4163,7 @@
         <v>111</v>
       </c>
       <c r="M25" s="33" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N25" s="36" t="s">
         <v>144</v>
@@ -4185,7 +4196,7 @@
         <v>111</v>
       </c>
       <c r="M26" s="23" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N26" s="5" t="s">
         <v>147</v>
@@ -4225,7 +4236,7 @@
         <v>111</v>
       </c>
       <c r="M27" s="33" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="N27" s="36" t="s">
         <v>149</v>
@@ -4268,7 +4279,7 @@
         <v>111</v>
       </c>
       <c r="M28" s="33" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="N28" s="36" t="s">
         <v>149</v>
@@ -4308,7 +4319,7 @@
         <v>111</v>
       </c>
       <c r="M29" s="33" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="N29" s="36" t="s">
         <v>149</v>
@@ -4348,7 +4359,7 @@
         <v>111</v>
       </c>
       <c r="M30" s="33" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="N30" s="36" t="s">
         <v>150</v>
@@ -4388,7 +4399,7 @@
         <v>111</v>
       </c>
       <c r="M31" s="33" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="N31" s="36" t="s">
         <v>151</v>
@@ -4411,7 +4422,7 @@
         <v>352</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="I32" s="5" t="b">
         <v>0</v>
@@ -4427,15 +4438,15 @@
         <v>111</v>
       </c>
       <c r="M32" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N32" s="5" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="33" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>56</v>
@@ -4450,7 +4461,7 @@
         <v>352</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="I33" s="5" t="b">
         <v>0</v>
@@ -4466,10 +4477,10 @@
         <v>111</v>
       </c>
       <c r="M33" s="23" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N33" s="5" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -4499,7 +4510,7 @@
         <v>111</v>
       </c>
       <c r="M34" s="23" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="N34" s="5" t="s">
         <v>149</v>
@@ -4540,7 +4551,7 @@
         <v>111</v>
       </c>
       <c r="M35" s="33" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="N35" s="36" t="s">
         <v>149</v>
@@ -4576,7 +4587,7 @@
         <v>111</v>
       </c>
       <c r="M36" s="23" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="N36" s="5" t="s">
         <v>149</v>
@@ -4612,7 +4623,7 @@
         <v>111</v>
       </c>
       <c r="M37" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N37" s="7" t="s">
         <v>123</v>
@@ -4655,7 +4666,7 @@
         <v>110</v>
       </c>
       <c r="M38" s="33" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N38" s="36" t="s">
         <v>137</v>
@@ -4698,7 +4709,7 @@
         <v>110</v>
       </c>
       <c r="M39" s="33" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N39" s="36" t="s">
         <v>137</v>
@@ -4741,7 +4752,7 @@
         <v>110</v>
       </c>
       <c r="M40" s="33" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N40" s="36" t="s">
         <v>136</v>
@@ -4784,7 +4795,7 @@
         <v>110</v>
       </c>
       <c r="M41" s="33" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N41" s="36" t="s">
         <v>136</v>
@@ -4827,7 +4838,7 @@
         <v>110</v>
       </c>
       <c r="M42" s="33" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N42" s="36" t="s">
         <v>135</v>
@@ -4870,7 +4881,7 @@
         <v>110</v>
       </c>
       <c r="M43" s="33" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N43" s="36" t="s">
         <v>135</v>
@@ -4913,7 +4924,7 @@
         <v>111</v>
       </c>
       <c r="M44" s="24" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N44" s="19" t="s">
         <v>123</v>
@@ -4921,7 +4932,7 @@
     </row>
     <row r="45" spans="1:14" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="15" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="B45" s="16" t="s">
         <v>56</v>
@@ -4956,7 +4967,7 @@
         <v>111</v>
       </c>
       <c r="M45" s="24" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N45" s="19" t="s">
         <v>123</v>
@@ -4999,7 +5010,7 @@
         <v>111</v>
       </c>
       <c r="M46" s="24" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N46" s="19" t="s">
         <v>123</v>
@@ -5035,7 +5046,7 @@
         <v>111</v>
       </c>
       <c r="M47" s="23" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="N47" s="7" t="s">
         <v>121</v>
@@ -5071,7 +5082,7 @@
         <v>111</v>
       </c>
       <c r="M48" s="23" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="N48" s="7" t="s">
         <v>122</v>
@@ -5107,7 +5118,7 @@
         <v>111</v>
       </c>
       <c r="M49" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N49" s="7" t="s">
         <v>123</v>
@@ -5143,7 +5154,7 @@
         <v>111</v>
       </c>
       <c r="M50" s="23" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N50" s="7" t="s">
         <v>123</v>
@@ -5183,7 +5194,7 @@
         <v>111</v>
       </c>
       <c r="M51" s="33" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="N51" s="36" t="s">
         <v>124</v>
@@ -5219,7 +5230,7 @@
         <v>111</v>
       </c>
       <c r="M52" s="23" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="N52" s="5" t="s">
         <v>125</v>
@@ -5255,7 +5266,7 @@
         <v>111</v>
       </c>
       <c r="M53" s="23" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="N53" s="7" t="s">
         <v>126</v>
@@ -5294,7 +5305,7 @@
         <v>111</v>
       </c>
       <c r="M54" s="23" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="N54" s="5" t="s">
         <v>481</v>
@@ -5317,7 +5328,7 @@
         <v>352</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="I55" s="5" t="b">
         <v>0</v>
@@ -5333,10 +5344,10 @@
         <v>111</v>
       </c>
       <c r="M55" s="23" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="N55" s="5" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="56" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -5369,7 +5380,7 @@
         <v>111</v>
       </c>
       <c r="M56" s="23" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="N56" s="7" t="s">
         <v>127</v>
@@ -5405,7 +5416,7 @@
         <v>111</v>
       </c>
       <c r="M57" s="23" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="N57" s="7" t="s">
         <v>128</v>
@@ -5441,7 +5452,7 @@
         <v>111</v>
       </c>
       <c r="M58" s="23" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="N58" s="7" t="s">
         <v>129</v>
@@ -5477,7 +5488,7 @@
         <v>111</v>
       </c>
       <c r="M59" s="23" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="N59" s="7" t="s">
         <v>130</v>
@@ -5513,7 +5524,7 @@
         <v>111</v>
       </c>
       <c r="M60" s="23" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="N60" s="7" t="s">
         <v>131</v>
@@ -5546,7 +5557,7 @@
         <v>111</v>
       </c>
       <c r="M61" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N61" s="7" t="s">
         <v>123</v>
@@ -5554,7 +5565,7 @@
     </row>
     <row r="62" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>56</v>
@@ -5579,7 +5590,7 @@
         <v>111</v>
       </c>
       <c r="M62" s="23" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N62" s="7" t="s">
         <v>123</v>
@@ -5615,7 +5626,7 @@
         <v>111</v>
       </c>
       <c r="M63" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N63" s="7" t="s">
         <v>123</v>
@@ -5658,7 +5669,7 @@
         <v>111</v>
       </c>
       <c r="M64" s="33" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N64" s="39" t="s">
         <v>123</v>
@@ -5697,7 +5708,7 @@
         <v>111</v>
       </c>
       <c r="M65" s="23" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N65" s="7" t="s">
         <v>123</v>
@@ -5740,7 +5751,7 @@
         <v>111</v>
       </c>
       <c r="M66" s="24" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N66" s="19" t="s">
         <v>123</v>
@@ -5748,7 +5759,7 @@
     </row>
     <row r="67" spans="1:14" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="15" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="B67" s="16" t="s">
         <v>56</v>
@@ -5783,7 +5794,7 @@
         <v>111</v>
       </c>
       <c r="M67" s="24" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N67" s="19" t="s">
         <v>123</v>
@@ -5826,7 +5837,7 @@
         <v>111</v>
       </c>
       <c r="M68" s="24" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N68" s="19" t="s">
         <v>123</v>
@@ -5862,7 +5873,7 @@
         <v>111</v>
       </c>
       <c r="M69" s="23" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N69" s="7" t="s">
         <v>132</v>
@@ -5898,7 +5909,7 @@
         <v>111</v>
       </c>
       <c r="M70" s="23" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N70" s="7" t="s">
         <v>133</v>
@@ -5934,7 +5945,7 @@
         <v>111</v>
       </c>
       <c r="M71" s="23" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="N71" s="7" t="s">
         <v>134</v>
@@ -5973,7 +5984,7 @@
         <v>111</v>
       </c>
       <c r="M72" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N72" s="7" t="s">
         <v>123</v>
@@ -5981,7 +5992,7 @@
     </row>
     <row r="73" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>56</v>
@@ -6012,7 +6023,7 @@
         <v>111</v>
       </c>
       <c r="M73" s="23" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N73" s="7" t="s">
         <v>123</v>
@@ -6048,7 +6059,7 @@
         <v>111</v>
       </c>
       <c r="M74" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N74" s="7" t="s">
         <v>234</v>
@@ -6056,7 +6067,7 @@
     </row>
     <row r="75" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="B75" s="4" t="s">
         <v>56</v>
@@ -6084,7 +6095,7 @@
         <v>111</v>
       </c>
       <c r="M75" s="23" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N75" s="7" t="s">
         <v>234</v>
@@ -6127,7 +6138,7 @@
         <v>111</v>
       </c>
       <c r="M76" s="24" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N76" s="19" t="s">
         <v>144</v>
@@ -6170,7 +6181,7 @@
         <v>111</v>
       </c>
       <c r="M77" s="24" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="N77" s="19" t="s">
         <v>143</v>
@@ -6213,7 +6224,7 @@
         <v>111</v>
       </c>
       <c r="M78" s="24" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N78" s="19" t="s">
         <v>123</v>
@@ -6221,7 +6232,7 @@
     </row>
     <row r="79" spans="1:14" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A79" s="15" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="B79" s="16" t="s">
         <v>56</v>
@@ -6256,7 +6267,7 @@
         <v>111</v>
       </c>
       <c r="M79" s="24" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N79" s="19" t="s">
         <v>123</v>
@@ -6299,7 +6310,7 @@
         <v>111</v>
       </c>
       <c r="M80" s="24" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N80" s="19" t="s">
         <v>123</v>
@@ -6335,7 +6346,7 @@
         <v>111</v>
       </c>
       <c r="M81" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N81" s="7" t="s">
         <v>123</v>
@@ -6343,7 +6354,7 @@
     </row>
     <row r="82" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="B82" s="4" t="s">
         <v>56</v>
@@ -6371,7 +6382,7 @@
         <v>111</v>
       </c>
       <c r="M82" s="23" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N82" s="7" t="s">
         <v>123</v>
@@ -6414,7 +6425,7 @@
         <v>111</v>
       </c>
       <c r="M83" s="24" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N83" s="19" t="s">
         <v>123</v>
@@ -6450,7 +6461,7 @@
         <v>111</v>
       </c>
       <c r="M84" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N84" s="7" t="s">
         <v>123</v>
@@ -6493,7 +6504,7 @@
         <v>111</v>
       </c>
       <c r="M85" s="24" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N85" s="19" t="s">
         <v>123</v>
@@ -6501,7 +6512,7 @@
     </row>
     <row r="86" spans="1:14" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A86" s="15" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="B86" s="16" t="s">
         <v>56</v>
@@ -6536,7 +6547,7 @@
         <v>111</v>
       </c>
       <c r="M86" s="24" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N86" s="19" t="s">
         <v>123</v>
@@ -6579,7 +6590,7 @@
         <v>111</v>
       </c>
       <c r="M87" s="24" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N87" s="19" t="s">
         <v>123</v>
@@ -6615,7 +6626,7 @@
         <v>111</v>
       </c>
       <c r="M88" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N88" s="7" t="s">
         <v>123</v>
@@ -6656,7 +6667,7 @@
         <v>111</v>
       </c>
       <c r="M89" s="33" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="N89" s="36" t="s">
         <v>177</v>
@@ -6697,7 +6708,7 @@
         <v>111</v>
       </c>
       <c r="M90" s="33" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="N90" s="36" t="s">
         <v>177</v>
@@ -6738,7 +6749,7 @@
         <v>111</v>
       </c>
       <c r="M91" s="33" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="N91" s="36" t="s">
         <v>177</v>
@@ -6779,7 +6790,7 @@
         <v>111</v>
       </c>
       <c r="M92" s="33" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="N92" s="36" t="s">
         <v>177</v>
@@ -6815,7 +6826,7 @@
         <v>111</v>
       </c>
       <c r="M93" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N93" s="5" t="s">
         <v>189</v>
@@ -6823,7 +6834,7 @@
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="B94" s="4" t="s">
         <v>56</v>
@@ -6851,7 +6862,7 @@
         <v>111</v>
       </c>
       <c r="M94" s="23" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N94" s="5" t="s">
         <v>189</v>
@@ -6887,7 +6898,7 @@
         <v>111</v>
       </c>
       <c r="M95" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N95" s="5" t="s">
         <v>189</v>
@@ -6923,7 +6934,7 @@
         <v>111</v>
       </c>
       <c r="M96" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N96" s="7" t="s">
         <v>123</v>
@@ -6931,7 +6942,7 @@
     </row>
     <row r="97" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="B97" s="4" t="s">
         <v>56</v>
@@ -6959,7 +6970,7 @@
         <v>111</v>
       </c>
       <c r="M97" s="23" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N97" s="7" t="s">
         <v>123</v>
@@ -7002,7 +7013,7 @@
         <v>111</v>
       </c>
       <c r="M98" s="24" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N98" s="19" t="s">
         <v>123</v>
@@ -7038,7 +7049,7 @@
         <v>111</v>
       </c>
       <c r="M99" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N99" s="7" t="s">
         <v>123</v>
@@ -7074,7 +7085,7 @@
         <v>111</v>
       </c>
       <c r="M100" s="23" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="N100" s="5" t="s">
         <v>235</v>
@@ -7110,7 +7121,7 @@
         <v>111</v>
       </c>
       <c r="M101" s="23" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="N101" s="7" t="s">
         <v>128</v>
@@ -7146,7 +7157,7 @@
         <v>111</v>
       </c>
       <c r="M102" s="23" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="N102" s="10" t="s">
         <v>213</v>
@@ -7187,7 +7198,7 @@
       <c r="K103" s="24"/>
       <c r="L103" s="24"/>
       <c r="M103" s="24" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="N103" s="19" t="s">
         <v>217</v>
@@ -7223,7 +7234,7 @@
         <v>111</v>
       </c>
       <c r="M104" s="23" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="N104" s="5" t="s">
         <v>410</v>
@@ -7259,7 +7270,7 @@
         <v>111</v>
       </c>
       <c r="M105" s="23" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="N105" s="5" t="s">
         <v>177</v>
@@ -7295,7 +7306,7 @@
         <v>111</v>
       </c>
       <c r="M106" s="23" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="N106" s="5" t="s">
         <v>177</v>
@@ -7331,7 +7342,7 @@
         <v>111</v>
       </c>
       <c r="M107" s="23" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="N107" s="5" t="s">
         <v>410</v>
@@ -7367,7 +7378,7 @@
         <v>349</v>
       </c>
       <c r="M108" s="25" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="N108" s="5" t="s">
         <v>406</v>
@@ -7403,7 +7414,7 @@
         <v>349</v>
       </c>
       <c r="M109" s="25" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="N109" s="5" t="s">
         <v>408</v>
@@ -7439,7 +7450,7 @@
         <v>349</v>
       </c>
       <c r="M110" s="25" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="N110" s="5" t="s">
         <v>408</v>
@@ -7475,7 +7486,7 @@
         <v>349</v>
       </c>
       <c r="M111" s="25" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="N111" s="5" t="s">
         <v>406</v>
@@ -7511,7 +7522,7 @@
         <v>349</v>
       </c>
       <c r="M112" s="25" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="N112" s="5" t="s">
         <v>409</v>
@@ -7547,7 +7558,7 @@
         <v>349</v>
       </c>
       <c r="M113" s="25" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="N113" s="5" t="s">
         <v>406</v>
@@ -7583,7 +7594,7 @@
         <v>349</v>
       </c>
       <c r="M114" s="25" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="N114" s="5" t="s">
         <v>406</v>
@@ -7619,7 +7630,7 @@
         <v>349</v>
       </c>
       <c r="M115" s="25" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="N115" s="5" t="s">
         <v>408</v>
@@ -7655,7 +7666,7 @@
         <v>349</v>
       </c>
       <c r="M116" s="25" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="N116" s="5" t="s">
         <v>409</v>
@@ -7691,7 +7702,7 @@
         <v>349</v>
       </c>
       <c r="M117" s="25" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="N117" s="5" t="s">
         <v>407</v>
@@ -7727,7 +7738,7 @@
         <v>349</v>
       </c>
       <c r="M118" s="25" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="N118" s="5" t="s">
         <v>407</v>
@@ -7763,7 +7774,7 @@
         <v>349</v>
       </c>
       <c r="M119" s="25" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="N119" s="5" t="s">
         <v>407</v>
@@ -7799,7 +7810,7 @@
         <v>349</v>
       </c>
       <c r="M120" s="25" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="N120" s="5" t="s">
         <v>407</v>
@@ -7835,7 +7846,7 @@
         <v>349</v>
       </c>
       <c r="M121" s="25" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="N121" s="5" t="s">
         <v>407</v>
@@ -7871,7 +7882,7 @@
         <v>349</v>
       </c>
       <c r="M122" s="25" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="N122" s="5" t="s">
         <v>407</v>
@@ -7907,7 +7918,7 @@
         <v>349</v>
       </c>
       <c r="M123" s="25" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="N123" s="5" t="s">
         <v>284</v>
@@ -7943,7 +7954,7 @@
         <v>349</v>
       </c>
       <c r="M124" s="25" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="N124" s="5" t="s">
         <v>285</v>
@@ -7979,7 +7990,7 @@
         <v>349</v>
       </c>
       <c r="M125" s="25" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="N125" s="5" t="s">
         <v>285</v>
@@ -8015,7 +8026,7 @@
         <v>349</v>
       </c>
       <c r="M126" s="25" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="N126" s="5" t="s">
         <v>285</v>
@@ -8051,7 +8062,7 @@
         <v>349</v>
       </c>
       <c r="M127" s="25" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="N127" s="5" t="s">
         <v>286</v>
@@ -8087,7 +8098,7 @@
         <v>349</v>
       </c>
       <c r="M128" s="25" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="N128" s="5" t="s">
         <v>286</v>
@@ -8123,7 +8134,7 @@
         <v>349</v>
       </c>
       <c r="M129" s="25" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="N129" s="5" t="s">
         <v>286</v>
@@ -8161,7 +8172,7 @@
         <v>110</v>
       </c>
       <c r="M130" s="23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N130" s="5" t="s">
         <v>290</v>
@@ -8199,7 +8210,7 @@
         <v>110</v>
       </c>
       <c r="M131" s="23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N131" s="5" t="s">
         <v>290</v>
@@ -8237,7 +8248,7 @@
         <v>110</v>
       </c>
       <c r="M132" s="23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N132" s="5" t="s">
         <v>291</v>
@@ -8275,7 +8286,7 @@
         <v>110</v>
       </c>
       <c r="M133" s="23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N133" s="5" t="s">
         <v>291</v>
@@ -8310,7 +8321,7 @@
         <v>111</v>
       </c>
       <c r="M134" s="23" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="N134" s="5" t="s">
         <v>141</v>
@@ -8345,7 +8356,7 @@
         <v>111</v>
       </c>
       <c r="M135" s="23" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="N135" s="5" t="s">
         <v>141</v>
@@ -8380,7 +8391,7 @@
         <v>111</v>
       </c>
       <c r="M136" s="23" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="N136" s="5" t="s">
         <v>149</v>
@@ -8415,7 +8426,7 @@
         <v>111</v>
       </c>
       <c r="M137" s="23" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="N137" s="5" t="s">
         <v>149</v>
@@ -8450,7 +8461,7 @@
         <v>111</v>
       </c>
       <c r="M138" s="23" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="N138" s="5" t="s">
         <v>150</v>
@@ -8485,7 +8496,7 @@
         <v>111</v>
       </c>
       <c r="M139" s="23" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="N139" s="5" t="s">
         <v>321</v>
@@ -8520,7 +8531,7 @@
         <v>111</v>
       </c>
       <c r="M140" s="23" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="N140" s="5" t="s">
         <v>322</v>
@@ -8555,7 +8566,7 @@
         <v>111</v>
       </c>
       <c r="M141" s="23" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="N141" s="5" t="s">
         <v>322</v>
@@ -8590,7 +8601,7 @@
         <v>111</v>
       </c>
       <c r="M142" s="23" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="N142" s="5" t="s">
         <v>323</v>
@@ -8625,7 +8636,7 @@
         <v>111</v>
       </c>
       <c r="M143" s="23" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="N143" s="5" t="s">
         <v>324</v>
@@ -8660,7 +8671,7 @@
         <v>111</v>
       </c>
       <c r="M144" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N144" s="5" t="s">
         <v>325</v>
@@ -8695,7 +8706,7 @@
         <v>111</v>
       </c>
       <c r="M145" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N145" s="5" t="s">
         <v>326</v>
@@ -8730,7 +8741,7 @@
         <v>111</v>
       </c>
       <c r="M146" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N146" s="5" t="s">
         <v>327</v>
@@ -8765,7 +8776,7 @@
         <v>111</v>
       </c>
       <c r="M147" s="23" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N147" s="5" t="s">
         <v>327</v>
@@ -8800,7 +8811,7 @@
         <v>111</v>
       </c>
       <c r="M148" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N148" s="7" t="s">
         <v>123</v>
@@ -8808,7 +8819,7 @@
     </row>
     <row r="149" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="B149" s="4" t="s">
         <v>56</v>
@@ -8835,7 +8846,7 @@
         <v>111</v>
       </c>
       <c r="M149" s="23" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N149" s="7" t="s">
         <v>123</v>
@@ -8870,7 +8881,7 @@
         <v>111</v>
       </c>
       <c r="M150" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N150" s="7" t="s">
         <v>123</v>
@@ -8905,7 +8916,7 @@
         <v>111</v>
       </c>
       <c r="M151" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N151" s="7" t="s">
         <v>123</v>
@@ -8913,7 +8924,7 @@
     </row>
     <row r="152" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A152" s="5" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="B152" s="4" t="s">
         <v>56</v>
@@ -8940,7 +8951,7 @@
         <v>111</v>
       </c>
       <c r="M152" s="23" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N152" s="7" t="s">
         <v>123</v>
@@ -8975,7 +8986,7 @@
         <v>111</v>
       </c>
       <c r="M153" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N153" s="7" t="s">
         <v>123</v>
@@ -9010,7 +9021,7 @@
         <v>111</v>
       </c>
       <c r="M154" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N154" s="5" t="s">
         <v>356</v>
@@ -9045,7 +9056,7 @@
         <v>111</v>
       </c>
       <c r="M155" s="23" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N155" s="5" t="s">
         <v>355</v>
@@ -9080,7 +9091,7 @@
         <v>111</v>
       </c>
       <c r="M156" s="23" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N156" s="5" t="s">
         <v>357</v>
@@ -9118,7 +9129,7 @@
         <v>110</v>
       </c>
       <c r="M157" s="23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N157" s="5" t="s">
         <v>391</v>
@@ -9156,7 +9167,7 @@
         <v>110</v>
       </c>
       <c r="M158" s="23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N158" s="5" t="s">
         <v>391</v>
@@ -9194,7 +9205,7 @@
         <v>110</v>
       </c>
       <c r="M159" s="23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N159" s="5" t="s">
         <v>392</v>
@@ -9232,7 +9243,7 @@
         <v>110</v>
       </c>
       <c r="M160" s="23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N160" s="5" t="s">
         <v>392</v>
@@ -9270,7 +9281,7 @@
         <v>110</v>
       </c>
       <c r="M161" s="23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N161" s="5" t="s">
         <v>393</v>
@@ -9308,7 +9319,7 @@
         <v>110</v>
       </c>
       <c r="M162" s="23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N162" s="5" t="s">
         <v>393</v>
@@ -9346,7 +9357,7 @@
         <v>110</v>
       </c>
       <c r="M163" s="23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N163" s="5" t="s">
         <v>394</v>
@@ -9384,7 +9395,7 @@
         <v>110</v>
       </c>
       <c r="M164" s="23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N164" s="5" t="s">
         <v>394</v>
@@ -9422,7 +9433,7 @@
         <v>110</v>
       </c>
       <c r="M165" s="23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N165" s="5" t="s">
         <v>395</v>
@@ -9460,7 +9471,7 @@
         <v>110</v>
       </c>
       <c r="M166" s="23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N166" s="5" t="s">
         <v>395</v>
@@ -9498,7 +9509,7 @@
         <v>110</v>
       </c>
       <c r="M167" s="23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N167" s="5" t="s">
         <v>396</v>
@@ -9536,7 +9547,7 @@
         <v>110</v>
       </c>
       <c r="M168" s="23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N168" s="5" t="s">
         <v>396</v>
@@ -9574,7 +9585,7 @@
         <v>110</v>
       </c>
       <c r="M169" s="23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N169" s="5" t="s">
         <v>397</v>
@@ -9612,7 +9623,7 @@
         <v>110</v>
       </c>
       <c r="M170" s="23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N170" s="5" t="s">
         <v>397</v>
@@ -9650,7 +9661,7 @@
         <v>110</v>
       </c>
       <c r="M171" s="23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N171" s="5" t="s">
         <v>398</v>
@@ -9688,7 +9699,7 @@
         <v>110</v>
       </c>
       <c r="M172" s="23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N172" s="5" t="s">
         <v>398</v>
@@ -9730,7 +9741,7 @@
         <v>110</v>
       </c>
       <c r="M173" s="33" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N173" s="36" t="s">
         <v>399</v>
@@ -9768,7 +9779,7 @@
         <v>110</v>
       </c>
       <c r="M174" s="23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N174" s="5" t="s">
         <v>399</v>
@@ -9803,7 +9814,7 @@
         <v>111</v>
       </c>
       <c r="M175" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N175" s="7" t="s">
         <v>123</v>
@@ -9811,7 +9822,7 @@
     </row>
     <row r="176" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A176" s="5" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="B176" s="4" t="s">
         <v>56</v>
@@ -9838,7 +9849,7 @@
         <v>111</v>
       </c>
       <c r="M176" s="23" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N176" s="7" t="s">
         <v>123</v>
@@ -9873,7 +9884,7 @@
         <v>111</v>
       </c>
       <c r="M177" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N177" s="7" t="s">
         <v>123</v>
@@ -9908,7 +9919,7 @@
         <v>111</v>
       </c>
       <c r="M178" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N178" s="7" t="s">
         <v>123</v>
@@ -9916,7 +9927,7 @@
     </row>
     <row r="179" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A179" s="5" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="B179" s="4" t="s">
         <v>56</v>
@@ -9943,7 +9954,7 @@
         <v>111</v>
       </c>
       <c r="M179" s="23" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N179" s="7" t="s">
         <v>123</v>
@@ -9978,7 +9989,7 @@
         <v>111</v>
       </c>
       <c r="M180" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N180" s="7" t="s">
         <v>123</v>
@@ -10018,7 +10029,7 @@
         <v>426</v>
       </c>
       <c r="M181" s="33" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="N181" s="36" t="s">
         <v>425</v>
@@ -10058,7 +10069,7 @@
         <v>426</v>
       </c>
       <c r="M182" s="33" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="N182" s="36" t="s">
         <v>425</v>
@@ -10081,7 +10092,7 @@
         <v>352</v>
       </c>
       <c r="H183" s="5" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="I183" s="5" t="b">
         <v>0</v>
@@ -10099,7 +10110,7 @@
         <v>432</v>
       </c>
       <c r="N183" s="43" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="184" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -10207,7 +10218,7 @@
         <v>111</v>
       </c>
       <c r="M186" s="23" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="N186" s="5" t="s">
         <v>438</v>
@@ -10242,7 +10253,7 @@
         <v>111</v>
       </c>
       <c r="M187" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N187" s="5" t="s">
         <v>123</v>
@@ -10265,13 +10276,13 @@
         <v>482</v>
       </c>
       <c r="F188" s="21" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="G188" s="18">
         <v>45565</v>
       </c>
       <c r="H188" s="15" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="I188" s="15" t="b">
         <v>0</v>
@@ -10287,7 +10298,7 @@
         <v>111</v>
       </c>
       <c r="M188" s="24" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N188" s="19" t="s">
         <v>123</v>
@@ -10325,7 +10336,7 @@
         <v>111</v>
       </c>
       <c r="M189" s="23" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="N189" s="5" t="s">
         <v>474</v>
@@ -10363,7 +10374,7 @@
         <v>111</v>
       </c>
       <c r="M190" s="23" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="N190" s="5" t="s">
         <v>474</v>
@@ -10401,7 +10412,7 @@
         <v>111</v>
       </c>
       <c r="M191" s="23" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="N191" s="5" t="s">
         <v>474</v>
@@ -10436,7 +10447,7 @@
         <v>111</v>
       </c>
       <c r="M192" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N192" s="7" t="s">
         <v>123</v>
@@ -10444,7 +10455,7 @@
     </row>
     <row r="193" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A193" s="5" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="B193" s="4" t="s">
         <v>56</v>
@@ -10471,7 +10482,7 @@
         <v>111</v>
       </c>
       <c r="M193" s="23" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N193" s="7" t="s">
         <v>123</v>
@@ -10506,7 +10517,7 @@
         <v>111</v>
       </c>
       <c r="M194" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N194" s="7" t="s">
         <v>123</v>
@@ -10541,7 +10552,7 @@
         <v>111</v>
       </c>
       <c r="M195" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N195" s="7" t="s">
         <v>123</v>
@@ -10549,7 +10560,7 @@
     </row>
     <row r="196" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A196" s="5" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="B196" s="4" t="s">
         <v>56</v>
@@ -10576,7 +10587,7 @@
         <v>111</v>
       </c>
       <c r="M196" s="23" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N196" s="7" t="s">
         <v>123</v>
@@ -10611,7 +10622,7 @@
         <v>111</v>
       </c>
       <c r="M197" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N197" s="7" t="s">
         <v>123</v>
@@ -10634,13 +10645,13 @@
         <v>482</v>
       </c>
       <c r="F198" s="21" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="G198" s="18">
         <v>45565</v>
       </c>
       <c r="H198" s="15" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="I198" s="15" t="b">
         <v>0</v>
@@ -10656,7 +10667,7 @@
         <v>111</v>
       </c>
       <c r="M198" s="24" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N198" s="19" t="s">
         <v>507</v>
@@ -10695,7 +10706,7 @@
         <v>110</v>
       </c>
       <c r="M199" s="23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N199" s="5" t="s">
         <v>517</v>
@@ -10734,7 +10745,7 @@
         <v>110</v>
       </c>
       <c r="M200" s="23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N200" s="5" t="s">
         <v>517</v>
@@ -10773,7 +10784,7 @@
         <v>110</v>
       </c>
       <c r="M201" s="23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N201" s="5" t="s">
         <v>517</v>
@@ -10812,7 +10823,7 @@
         <v>110</v>
       </c>
       <c r="M202" s="23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N202" s="5" t="s">
         <v>517</v>
@@ -10850,7 +10861,7 @@
         <v>110</v>
       </c>
       <c r="M203" s="23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N203" s="5" t="s">
         <v>522</v>
@@ -10888,7 +10899,7 @@
         <v>110</v>
       </c>
       <c r="M204" s="23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N204" s="5" t="s">
         <v>522</v>
@@ -10926,7 +10937,7 @@
         <v>110</v>
       </c>
       <c r="M205" s="23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N205" s="5" t="s">
         <v>527</v>
@@ -10964,7 +10975,7 @@
         <v>110</v>
       </c>
       <c r="M206" s="23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N206" s="5" t="s">
         <v>527</v>
@@ -11002,7 +11013,7 @@
         <v>110</v>
       </c>
       <c r="M207" s="23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N207" s="5" t="s">
         <v>532</v>
@@ -11040,7 +11051,7 @@
         <v>110</v>
       </c>
       <c r="M208" s="23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N208" s="5" t="s">
         <v>532</v>
@@ -11078,7 +11089,7 @@
         <v>110</v>
       </c>
       <c r="M209" s="23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N209" s="5" t="s">
         <v>537</v>
@@ -11116,7 +11127,7 @@
         <v>110</v>
       </c>
       <c r="M210" s="23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N210" s="5" t="s">
         <v>537</v>
@@ -11154,7 +11165,7 @@
         <v>110</v>
       </c>
       <c r="M211" s="23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N211" s="5" t="s">
         <v>545</v>
@@ -11192,7 +11203,7 @@
         <v>110</v>
       </c>
       <c r="M212" s="23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N212" s="5" t="s">
         <v>550</v>
@@ -11230,7 +11241,7 @@
         <v>110</v>
       </c>
       <c r="M213" s="23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="N213" s="5" t="s">
         <v>550</v>
@@ -11493,7 +11504,7 @@
         <v>580</v>
       </c>
       <c r="M220" s="23" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="N220" s="5" t="s">
         <v>579</v>
@@ -11528,7 +11539,7 @@
         <v>426</v>
       </c>
       <c r="M221" s="23" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="N221" s="5" t="s">
         <v>586</v>
@@ -11563,7 +11574,7 @@
         <v>426</v>
       </c>
       <c r="M222" s="23" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="N222" s="5" t="s">
         <v>586</v>
@@ -11601,7 +11612,7 @@
         <v>111</v>
       </c>
       <c r="M223" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N223" s="5" t="s">
         <v>591</v>
@@ -11609,7 +11620,7 @@
     </row>
     <row r="224" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A224" s="5" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="B224" s="5" t="s">
         <v>588</v>
@@ -11639,7 +11650,7 @@
         <v>111</v>
       </c>
       <c r="M224" s="23" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N224" s="5" t="s">
         <v>591</v>
@@ -11662,13 +11673,13 @@
         <v>482</v>
       </c>
       <c r="F225" s="21" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="G225" s="18">
         <v>45565</v>
       </c>
       <c r="H225" s="15" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="I225" s="15" t="b">
         <v>0</v>
@@ -11683,7 +11694,7 @@
         <v>111</v>
       </c>
       <c r="M225" s="24" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N225" s="15" t="s">
         <v>591</v>
@@ -11721,7 +11732,7 @@
         <v>111</v>
       </c>
       <c r="M226" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N226" s="5" t="s">
         <v>591</v>
@@ -11759,7 +11770,7 @@
         <v>111</v>
       </c>
       <c r="M227" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N227" s="5" t="s">
         <v>507</v>
@@ -11782,13 +11793,13 @@
         <v>482</v>
       </c>
       <c r="F228" s="21" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="G228" s="18">
         <v>45565</v>
       </c>
       <c r="H228" s="15" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="I228" s="15" t="b">
         <v>0</v>
@@ -11803,7 +11814,7 @@
         <v>111</v>
       </c>
       <c r="M228" s="24" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N228" s="15" t="s">
         <v>591</v>
@@ -11841,7 +11852,7 @@
         <v>111</v>
       </c>
       <c r="M229" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N229" s="5" t="s">
         <v>591</v>
@@ -11861,7 +11872,7 @@
         <v>569</v>
       </c>
       <c r="E230" s="47" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="F230" s="48">
         <v>45792</v>
@@ -11870,7 +11881,7 @@
         <v>45870</v>
       </c>
       <c r="H230" s="45" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="I230" s="45" t="b">
         <v>0</v>
@@ -11885,7 +11896,7 @@
         <v>111</v>
       </c>
       <c r="M230" s="47" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N230" s="45" t="s">
         <v>591</v>
@@ -11905,7 +11916,7 @@
         <v>569</v>
       </c>
       <c r="E231" s="47" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="F231" s="48">
         <v>45792</v>
@@ -11914,7 +11925,7 @@
         <v>45870</v>
       </c>
       <c r="H231" s="45" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="I231" s="45" t="b">
         <v>0</v>
@@ -11929,7 +11940,7 @@
         <v>111</v>
       </c>
       <c r="M231" s="47" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N231" s="45" t="s">
         <v>591</v>
@@ -11949,7 +11960,7 @@
         <v>569</v>
       </c>
       <c r="E232" s="47" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="F232" s="48">
         <v>45792</v>
@@ -11958,7 +11969,7 @@
         <v>45870</v>
       </c>
       <c r="H232" s="45" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="I232" s="45" t="b">
         <v>0</v>
@@ -11973,7 +11984,7 @@
         <v>111</v>
       </c>
       <c r="M232" s="47" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N232" s="45" t="s">
         <v>507</v>
@@ -11993,7 +12004,7 @@
         <v>569</v>
       </c>
       <c r="E233" s="47" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="F233" s="48">
         <v>45792</v>
@@ -12002,7 +12013,7 @@
         <v>45870</v>
       </c>
       <c r="H233" s="45" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="I233" s="45" t="b">
         <v>0</v>
@@ -12017,7 +12028,7 @@
         <v>111</v>
       </c>
       <c r="M233" s="47" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N233" s="45" t="s">
         <v>507</v>
@@ -12055,7 +12066,7 @@
         <v>111</v>
       </c>
       <c r="M234" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N234" s="5" t="s">
         <v>591</v>
@@ -12093,7 +12104,7 @@
         <v>111</v>
       </c>
       <c r="M235" s="23" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N235" s="5" t="s">
         <v>591</v>
@@ -12131,7 +12142,7 @@
         <v>111</v>
       </c>
       <c r="M236" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N236" s="5" t="s">
         <v>507</v>
@@ -12169,7 +12180,7 @@
         <v>111</v>
       </c>
       <c r="M237" s="23" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N237" s="5" t="s">
         <v>507</v>
@@ -12204,7 +12215,7 @@
         <v>111</v>
       </c>
       <c r="M238" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N238" s="7" t="s">
         <v>123</v>
@@ -12212,7 +12223,7 @@
     </row>
     <row r="239" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A239" s="5" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="B239" s="4" t="s">
         <v>56</v>
@@ -12239,7 +12250,7 @@
         <v>111</v>
       </c>
       <c r="M239" s="23" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N239" s="7" t="s">
         <v>123</v>
@@ -12274,7 +12285,7 @@
         <v>111</v>
       </c>
       <c r="M240" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N240" s="7" t="s">
         <v>123</v>
@@ -12309,7 +12320,7 @@
         <v>111</v>
       </c>
       <c r="M241" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N241" s="7" t="s">
         <v>123</v>
@@ -12317,7 +12328,7 @@
     </row>
     <row r="242" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A242" s="5" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="B242" s="4" t="s">
         <v>56</v>
@@ -12344,7 +12355,7 @@
         <v>111</v>
       </c>
       <c r="M242" s="23" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N242" s="7" t="s">
         <v>123</v>
@@ -12379,7 +12390,7 @@
         <v>111</v>
       </c>
       <c r="M243" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N243" s="7" t="s">
         <v>123</v>
@@ -12417,7 +12428,7 @@
         <v>111</v>
       </c>
       <c r="M244" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N244" s="5" t="s">
         <v>591</v>
@@ -12455,7 +12466,7 @@
         <v>111</v>
       </c>
       <c r="M245" s="23" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N245" s="5" t="s">
         <v>591</v>
@@ -12493,7 +12504,7 @@
         <v>111</v>
       </c>
       <c r="M246" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N246" s="5" t="s">
         <v>591</v>
@@ -12531,7 +12542,7 @@
         <v>111</v>
       </c>
       <c r="M247" s="23" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N247" s="5" t="s">
         <v>591</v>
@@ -12569,7 +12580,7 @@
         <v>111</v>
       </c>
       <c r="M248" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N248" s="5" t="s">
         <v>507</v>
@@ -12607,182 +12618,206 @@
         <v>111</v>
       </c>
       <c r="M249" s="23" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N249" s="5" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="250" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A250" t="s">
+    <row r="250" spans="1:14" s="45" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A250" s="49" t="s">
         <v>633</v>
       </c>
-      <c r="B250" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C250" s="1" t="s">
+      <c r="B250" s="50" t="s">
+        <v>56</v>
+      </c>
+      <c r="C250" s="51" t="s">
         <v>637</v>
       </c>
-      <c r="D250" s="28" t="s">
+      <c r="D250" s="52" t="s">
         <v>631</v>
       </c>
-      <c r="E250" s="23" t="s">
-        <v>352</v>
-      </c>
-      <c r="H250" s="5" t="s">
-        <v>642</v>
-      </c>
-      <c r="I250" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="J250" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K250" s="23">
+      <c r="E250" s="47" t="s">
+        <v>779</v>
+      </c>
+      <c r="F250" s="48">
+        <v>45792</v>
+      </c>
+      <c r="G250" s="48">
+        <v>45817</v>
+      </c>
+      <c r="H250" s="45" t="s">
+        <v>780</v>
+      </c>
+      <c r="I250" s="45" t="b">
+        <v>0</v>
+      </c>
+      <c r="J250" s="45" t="b">
+        <v>1</v>
+      </c>
+      <c r="K250" s="47">
         <v>3</v>
       </c>
-      <c r="L250" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="M250" s="23" t="s">
+      <c r="L250" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="M250" s="47" t="s">
+        <v>693</v>
+      </c>
+      <c r="N250" s="45" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="251" spans="1:14" s="45" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A251" s="49" t="s">
+        <v>634</v>
+      </c>
+      <c r="B251" s="50" t="s">
+        <v>56</v>
+      </c>
+      <c r="C251" s="51" t="s">
+        <v>638</v>
+      </c>
+      <c r="D251" s="52" t="s">
+        <v>631</v>
+      </c>
+      <c r="E251" s="47" t="s">
+        <v>779</v>
+      </c>
+      <c r="F251" s="48">
+        <v>45792</v>
+      </c>
+      <c r="G251" s="48">
+        <v>45817</v>
+      </c>
+      <c r="H251" s="45" t="s">
+        <v>780</v>
+      </c>
+      <c r="I251" s="45" t="b">
+        <v>0</v>
+      </c>
+      <c r="J251" s="45" t="b">
+        <v>1</v>
+      </c>
+      <c r="K251" s="47">
+        <v>3</v>
+      </c>
+      <c r="L251" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="M251" s="47" t="s">
         <v>694</v>
       </c>
-      <c r="N250" s="5" t="s">
+      <c r="N251" s="45" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="251" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A251" t="s">
-        <v>634</v>
-      </c>
-      <c r="B251" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C251" s="1" t="s">
-        <v>638</v>
-      </c>
-      <c r="D251" s="28" t="s">
+    <row r="252" spans="1:14" s="45" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A252" s="49" t="s">
+        <v>635</v>
+      </c>
+      <c r="B252" s="50" t="s">
+        <v>56</v>
+      </c>
+      <c r="C252" s="51" t="s">
+        <v>639</v>
+      </c>
+      <c r="D252" s="52" t="s">
         <v>631</v>
       </c>
-      <c r="E251" s="23" t="s">
-        <v>352</v>
-      </c>
-      <c r="H251" s="5" t="s">
-        <v>642</v>
-      </c>
-      <c r="I251" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="J251" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K251" s="23">
+      <c r="E252" s="47" t="s">
+        <v>779</v>
+      </c>
+      <c r="F252" s="48">
+        <v>45792</v>
+      </c>
+      <c r="G252" s="48">
+        <v>45817</v>
+      </c>
+      <c r="H252" s="45" t="s">
+        <v>780</v>
+      </c>
+      <c r="I252" s="45" t="b">
+        <v>0</v>
+      </c>
+      <c r="J252" s="45" t="b">
+        <v>1</v>
+      </c>
+      <c r="K252" s="47">
         <v>3</v>
       </c>
-      <c r="L251" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="M251" s="23" t="s">
-        <v>695</v>
-      </c>
-      <c r="N251" s="5" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="252" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A252" t="s">
-        <v>635</v>
-      </c>
-      <c r="B252" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C252" s="1" t="s">
-        <v>639</v>
-      </c>
-      <c r="D252" s="28" t="s">
+      <c r="L252" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="M252" s="47" t="s">
+        <v>693</v>
+      </c>
+      <c r="N252" s="45" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="253" spans="1:14" s="45" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A253" s="49" t="s">
+        <v>636</v>
+      </c>
+      <c r="B253" s="50" t="s">
+        <v>56</v>
+      </c>
+      <c r="C253" s="51" t="s">
+        <v>640</v>
+      </c>
+      <c r="D253" s="52" t="s">
         <v>631</v>
       </c>
-      <c r="E252" s="23" t="s">
-        <v>352</v>
-      </c>
-      <c r="H252" s="5" t="s">
-        <v>642</v>
-      </c>
-      <c r="I252" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="J252" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K252" s="23">
+      <c r="E253" s="47" t="s">
+        <v>779</v>
+      </c>
+      <c r="F253" s="48">
+        <v>45792</v>
+      </c>
+      <c r="G253" s="48">
+        <v>45817</v>
+      </c>
+      <c r="H253" s="45" t="s">
+        <v>780</v>
+      </c>
+      <c r="I253" s="45" t="b">
+        <v>0</v>
+      </c>
+      <c r="J253" s="45" t="b">
+        <v>1</v>
+      </c>
+      <c r="K253" s="47">
         <v>3</v>
       </c>
-      <c r="L252" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="M252" s="23" t="s">
+      <c r="L253" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="M253" s="47" t="s">
         <v>694</v>
       </c>
-      <c r="N252" s="5" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="253" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A253" t="s">
-        <v>636</v>
-      </c>
-      <c r="B253" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C253" s="1" t="s">
-        <v>640</v>
-      </c>
-      <c r="D253" s="28" t="s">
-        <v>631</v>
-      </c>
-      <c r="E253" s="23" t="s">
-        <v>352</v>
-      </c>
-      <c r="H253" s="5" t="s">
-        <v>642</v>
-      </c>
-      <c r="I253" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="J253" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K253" s="23">
-        <v>3</v>
-      </c>
-      <c r="L253" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="M253" s="23" t="s">
-        <v>695</v>
-      </c>
-      <c r="N253" s="5" t="s">
+      <c r="N253" s="45" t="s">
         <v>507</v>
       </c>
     </row>
     <row r="254" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A254" s="5" t="s">
+        <v>643</v>
+      </c>
+      <c r="B254" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C254" t="s">
+        <v>647</v>
+      </c>
+      <c r="D254" s="27" t="s">
         <v>644</v>
       </c>
-      <c r="B254" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C254" t="s">
-        <v>648</v>
-      </c>
-      <c r="D254" s="27" t="s">
-        <v>645</v>
-      </c>
       <c r="E254" s="23" t="s">
         <v>352</v>
       </c>
       <c r="H254" s="5" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="I254" s="5" t="b">
         <v>0</v>
@@ -12794,30 +12829,30 @@
         <v>580</v>
       </c>
       <c r="M254" s="23" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="N254" s="5" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="255" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A255" s="5" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B255" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C255" s="5" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D255" s="27" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="E255" s="23" t="s">
         <v>352</v>
       </c>
       <c r="H255" s="5" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="I255" s="5" t="b">
         <v>0</v>
@@ -12829,30 +12864,30 @@
         <v>580</v>
       </c>
       <c r="M255" s="23" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="N255" s="5" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="256" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A256" s="5" t="s">
+        <v>649</v>
+      </c>
+      <c r="B256" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C256" s="5" t="s">
         <v>650</v>
       </c>
-      <c r="B256" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C256" s="5" t="s">
-        <v>651</v>
-      </c>
       <c r="D256" s="27" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="E256" s="23" t="s">
         <v>352</v>
       </c>
       <c r="H256" s="5" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="I256" s="5" t="b">
         <v>0</v>
@@ -12864,30 +12899,30 @@
         <v>580</v>
       </c>
       <c r="M256" s="23" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="N256" s="5" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="257" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A257" s="5" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B257" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C257" s="5" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="D257" s="27" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="E257" s="23" t="s">
         <v>352</v>
       </c>
       <c r="H257" s="5" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="I257" s="5" t="b">
         <v>0</v>
@@ -12899,30 +12934,30 @@
         <v>580</v>
       </c>
       <c r="M257" s="23" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="N257" s="5" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="258" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A258" s="5" t="s">
+        <v>652</v>
+      </c>
+      <c r="B258" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C258" s="5" t="s">
         <v>653</v>
       </c>
-      <c r="B258" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C258" s="5" t="s">
-        <v>654</v>
-      </c>
       <c r="D258" s="27" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="E258" s="23" t="s">
         <v>352</v>
       </c>
       <c r="H258" s="5" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="I258" s="5" t="b">
         <v>0</v>
@@ -12934,30 +12969,30 @@
         <v>580</v>
       </c>
       <c r="M258" s="23" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="N258" s="5" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="259" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A259" s="5" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B259" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C259" s="5" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="D259" s="27" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="E259" s="23" t="s">
         <v>352</v>
       </c>
       <c r="H259" s="5" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="I259" s="5" t="b">
         <v>0</v>
@@ -12969,30 +13004,30 @@
         <v>580</v>
       </c>
       <c r="M259" s="23" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="N259" s="5" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="260" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A260" s="5" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B260" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C260" s="5" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="D260" s="27" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="E260" s="23" t="s">
         <v>352</v>
       </c>
       <c r="H260" s="5" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I260" s="5" t="b">
         <v>0</v>
@@ -13004,30 +13039,30 @@
         <v>580</v>
       </c>
       <c r="M260" s="23" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="N260" s="5" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="261" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A261" s="5" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B261" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C261" s="5" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D261" s="27" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="E261" s="23" t="s">
         <v>352</v>
       </c>
       <c r="H261" s="5" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I261" s="5" t="b">
         <v>0</v>
@@ -13039,30 +13074,30 @@
         <v>580</v>
       </c>
       <c r="M261" s="23" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="N261" s="5" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="262" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A262" s="5" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B262" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C262" s="5" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D262" s="27" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="E262" s="23" t="s">
         <v>352</v>
       </c>
       <c r="H262" s="5" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I262" s="5" t="b">
         <v>0</v>
@@ -13074,30 +13109,30 @@
         <v>580</v>
       </c>
       <c r="M262" s="23" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="N262" s="5" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="263" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A263" s="5" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B263" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C263" s="5" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="D263" s="27" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="E263" s="23" t="s">
         <v>352</v>
       </c>
       <c r="H263" s="5" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I263" s="5" t="b">
         <v>0</v>
@@ -13109,30 +13144,30 @@
         <v>580</v>
       </c>
       <c r="M263" s="23" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="N263" s="5" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="264" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A264" s="5" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B264" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C264" s="5" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="D264" s="27" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="E264" s="23" t="s">
         <v>352</v>
       </c>
       <c r="H264" s="5" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I264" s="5" t="b">
         <v>0</v>
@@ -13144,30 +13179,30 @@
         <v>580</v>
       </c>
       <c r="M264" s="23" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="N264" s="5" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="265" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A265" s="5" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B265" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C265" s="5" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="D265" s="27" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="E265" s="23" t="s">
         <v>352</v>
       </c>
       <c r="H265" s="5" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I265" s="5" t="b">
         <v>0</v>
@@ -13179,30 +13214,30 @@
         <v>580</v>
       </c>
       <c r="M265" s="23" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="N265" s="5" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="266" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A266" s="5" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B266" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C266" s="5" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="D266" s="27" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="E266" s="23" t="s">
         <v>352</v>
       </c>
       <c r="H266" s="5" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I266" s="5" t="b">
         <v>0</v>
@@ -13214,30 +13249,30 @@
         <v>580</v>
       </c>
       <c r="M266" s="23" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="N266" s="5" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="267" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A267" s="5" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B267" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C267" s="5" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="D267" s="27" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="E267" s="23" t="s">
         <v>352</v>
       </c>
       <c r="H267" s="5" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I267" s="5" t="b">
         <v>0</v>
@@ -13249,30 +13284,30 @@
         <v>580</v>
       </c>
       <c r="M267" s="23" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="N267" s="5" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="268" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A268" s="5" t="s">
+        <v>679</v>
+      </c>
+      <c r="B268" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C268" s="5" t="s">
+        <v>670</v>
+      </c>
+      <c r="D268" s="27" t="s">
+        <v>644</v>
+      </c>
+      <c r="E268" s="23" t="s">
+        <v>352</v>
+      </c>
+      <c r="H268" s="5" t="s">
         <v>680</v>
-      </c>
-      <c r="B268" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C268" s="5" t="s">
-        <v>671</v>
-      </c>
-      <c r="D268" s="27" t="s">
-        <v>645</v>
-      </c>
-      <c r="E268" s="23" t="s">
-        <v>352</v>
-      </c>
-      <c r="H268" s="5" t="s">
-        <v>681</v>
       </c>
       <c r="I268" s="5" t="b">
         <v>0</v>
@@ -13284,30 +13319,30 @@
         <v>580</v>
       </c>
       <c r="M268" s="23" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="N268" s="5" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="269" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A269" s="5" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B269" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C269" s="5" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D269" s="27" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="E269" s="23" t="s">
         <v>352</v>
       </c>
       <c r="H269" s="5" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="I269" s="5" t="b">
         <v>0</v>
@@ -13323,30 +13358,30 @@
         <v>111</v>
       </c>
       <c r="M269" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N269" s="5" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="270" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A270" s="5" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="B270" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C270" s="5" t="s">
+        <v>710</v>
+      </c>
+      <c r="D270" s="27" t="s">
         <v>711</v>
       </c>
-      <c r="D270" s="27" t="s">
-        <v>712</v>
-      </c>
       <c r="E270" s="23" t="s">
         <v>352</v>
       </c>
       <c r="H270" s="5" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="I270" s="5" t="b">
         <v>0</v>
@@ -13362,30 +13397,30 @@
         <v>111</v>
       </c>
       <c r="M270" s="23" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N270" s="5" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="271" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A271" s="5" t="s">
+        <v>714</v>
+      </c>
+      <c r="B271" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C271" s="5" t="s">
+        <v>712</v>
+      </c>
+      <c r="D271" s="27" t="s">
+        <v>711</v>
+      </c>
+      <c r="E271" s="23" t="s">
+        <v>352</v>
+      </c>
+      <c r="H271" s="5" t="s">
         <v>715</v>
-      </c>
-      <c r="B271" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C271" s="5" t="s">
-        <v>713</v>
-      </c>
-      <c r="D271" s="27" t="s">
-        <v>712</v>
-      </c>
-      <c r="E271" s="23" t="s">
-        <v>352</v>
-      </c>
-      <c r="H271" s="5" t="s">
-        <v>716</v>
       </c>
       <c r="I271" s="5" t="b">
         <v>0</v>
@@ -13397,30 +13432,30 @@
         <v>580</v>
       </c>
       <c r="M271" s="23" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="N271" s="5" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="272" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A272" s="5" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B272" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C272" s="5" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="D272" s="27" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="E272" s="23" t="s">
         <v>352</v>
       </c>
       <c r="H272" s="5" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="I272" s="5" t="b">
         <v>0</v>
@@ -13433,33 +13468,33 @@
         <v>1</v>
       </c>
       <c r="L272" s="23" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="M272" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N272" s="5" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="273" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A273" s="5" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B273" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C273" s="5" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="D273" s="27" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="E273" s="23" t="s">
         <v>352</v>
       </c>
       <c r="H273" s="5" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="I273" s="5" t="b">
         <v>0</v>
@@ -13472,33 +13507,33 @@
         <v>1</v>
       </c>
       <c r="L273" s="23" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="M273" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N273" s="5" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="274" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A274" s="5" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B274" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C274" s="5" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="D274" s="27" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="E274" s="23" t="s">
         <v>352</v>
       </c>
       <c r="H274" s="5" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="I274" s="5" t="b">
         <v>0</v>
@@ -13511,33 +13546,33 @@
         <v>1</v>
       </c>
       <c r="L274" s="23" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="M274" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N274" s="5" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="275" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A275" s="5" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B275" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C275" s="5" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="D275" s="27" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="E275" s="23" t="s">
         <v>352</v>
       </c>
       <c r="H275" s="5" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="I275" s="5" t="b">
         <v>0</v>
@@ -13550,33 +13585,33 @@
         <v>1</v>
       </c>
       <c r="L275" s="23" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="M275" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N275" s="5" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="276" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A276" s="5" t="s">
+        <v>726</v>
+      </c>
+      <c r="B276" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C276" s="5" t="s">
         <v>727</v>
       </c>
-      <c r="B276" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C276" s="5" t="s">
-        <v>728</v>
-      </c>
       <c r="D276" s="27" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="E276" s="23" t="s">
         <v>352</v>
       </c>
       <c r="H276" s="5" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="I276" s="5" t="b">
         <v>0</v>
@@ -13589,33 +13624,33 @@
         <v>1</v>
       </c>
       <c r="L276" s="23" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="M276" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N276" s="5" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="277" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A277" s="5" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B277" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C277" s="5" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="D277" s="27" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="E277" s="23" t="s">
         <v>352</v>
       </c>
       <c r="H277" s="5" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="I277" s="5" t="b">
         <v>0</v>
@@ -13628,33 +13663,33 @@
         <v>1</v>
       </c>
       <c r="L277" s="23" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="M277" s="23" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="N277" s="5" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="278" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A278" s="5" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="B278" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C278" s="5" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="D278" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="E278" s="23" t="s">
+        <v>352</v>
+      </c>
+      <c r="H278" s="5" t="s">
         <v>741</v>
-      </c>
-      <c r="E278" s="23" t="s">
-        <v>352</v>
-      </c>
-      <c r="H278" s="5" t="s">
-        <v>742</v>
       </c>
       <c r="I278" s="5" t="b">
         <v>0</v>
@@ -13667,33 +13702,33 @@
         <v>1</v>
       </c>
       <c r="L278" s="23" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="M278" s="23" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N278" s="5" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="279" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A279" s="5" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="B279" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C279" s="5" t="s">
+        <v>739</v>
+      </c>
+      <c r="D279" s="28" t="s">
         <v>740</v>
       </c>
-      <c r="D279" s="28" t="s">
+      <c r="E279" s="23" t="s">
+        <v>352</v>
+      </c>
+      <c r="H279" s="5" t="s">
         <v>741</v>
-      </c>
-      <c r="E279" s="23" t="s">
-        <v>352</v>
-      </c>
-      <c r="H279" s="5" t="s">
-        <v>742</v>
       </c>
       <c r="I279" s="5" t="b">
         <v>0</v>
@@ -13706,33 +13741,33 @@
         <v>1</v>
       </c>
       <c r="L279" s="23" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="M279" s="23" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N279" s="5" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="280" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="B280" s="5" t="s">
         <v>588</v>
       </c>
       <c r="C280" s="1" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="D280" s="28" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E280" s="23" t="s">
         <v>352</v>
       </c>
       <c r="H280" s="5" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="I280" s="5" t="b">
         <v>0</v>
@@ -13748,7 +13783,7 @@
         <v>111</v>
       </c>
       <c r="M280" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N280" s="5" t="s">
         <v>591</v>
@@ -13756,22 +13791,22 @@
     </row>
     <row r="281" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B281" s="5" t="s">
         <v>588</v>
       </c>
       <c r="C281" s="1" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="D281" s="28" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E281" s="23" t="s">
         <v>352</v>
       </c>
       <c r="H281" s="5" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="I281" s="5" t="b">
         <v>0</v>
@@ -13787,7 +13822,7 @@
         <v>111</v>
       </c>
       <c r="M281" s="23" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N281" s="5" t="s">
         <v>591</v>
@@ -13795,22 +13830,22 @@
     </row>
     <row r="282" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="B282" s="5" t="s">
         <v>588</v>
       </c>
       <c r="C282" s="1" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="D282" s="28" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E282" s="23" t="s">
         <v>352</v>
       </c>
       <c r="H282" s="5" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="I282" s="5" t="b">
         <v>0</v>
@@ -13826,7 +13861,7 @@
         <v>111</v>
       </c>
       <c r="M282" s="23" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="N282" s="5" t="s">
         <v>507</v>
@@ -13834,22 +13869,22 @@
     </row>
     <row r="283" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B283" s="5" t="s">
         <v>588</v>
       </c>
       <c r="C283" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="D283" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="E283" s="23" t="s">
+        <v>352</v>
+      </c>
+      <c r="H283" s="5" t="s">
         <v>750</v>
-      </c>
-      <c r="D283" s="28" t="s">
-        <v>741</v>
-      </c>
-      <c r="E283" s="23" t="s">
-        <v>352</v>
-      </c>
-      <c r="H283" s="5" t="s">
-        <v>751</v>
       </c>
       <c r="I283" s="5" t="b">
         <v>0</v>
@@ -13865,7 +13900,7 @@
         <v>111</v>
       </c>
       <c r="M283" s="23" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N283" s="5" t="s">
         <v>507</v>

</xml_diff>

<commit_message>
Updated A-NZ removal dates
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Document types v9.1.xlsx
+++ b/work-in-progress/Peppol Code Lists - Document types v9.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\peppol-edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC42692-FB72-4D61-94CD-3C1D06F73239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D30077CD-8446-45DE-B11A-455823A18F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17895" yWindow="135" windowWidth="25560" windowHeight="20745" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Document Type" sheetId="5" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2478" uniqueCount="781">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2482" uniqueCount="781">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -2579,7 +2579,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2705,9 +2705,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -3141,8 +3138,8 @@
   <dimension ref="A1:N283"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A262" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A283" sqref="A283"/>
+      <pane ySplit="1" topLeftCell="A222" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A233" sqref="A233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11858,179 +11855,179 @@
         <v>591</v>
       </c>
     </row>
-    <row r="230" spans="1:14" s="45" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A230" s="45" t="s">
+    <row r="230" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A230" s="36" t="s">
         <v>598</v>
       </c>
-      <c r="B230" s="45" t="s">
-        <v>56</v>
-      </c>
-      <c r="C230" s="45" t="s">
+      <c r="B230" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="C230" s="36" t="s">
         <v>599</v>
       </c>
-      <c r="D230" s="46" t="s">
+      <c r="D230" s="32" t="s">
         <v>569</v>
       </c>
-      <c r="E230" s="47" t="s">
-        <v>779</v>
-      </c>
-      <c r="F230" s="48">
-        <v>45792</v>
-      </c>
-      <c r="G230" s="48">
-        <v>45870</v>
-      </c>
-      <c r="H230" s="45" t="s">
+      <c r="E230" s="33" t="s">
+        <v>351</v>
+      </c>
+      <c r="F230" s="41" t="s">
+        <v>740</v>
+      </c>
+      <c r="G230" s="35">
+        <v>45717</v>
+      </c>
+      <c r="H230" s="36" t="s">
         <v>751</v>
       </c>
-      <c r="I230" s="45" t="b">
-        <v>0</v>
-      </c>
-      <c r="J230" s="45" t="b">
-        <v>1</v>
-      </c>
-      <c r="K230" s="47">
+      <c r="I230" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="J230" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="K230" s="33">
         <v>3</v>
       </c>
-      <c r="L230" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="M230" s="47" t="s">
+      <c r="L230" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="M230" s="33" t="s">
         <v>693</v>
       </c>
-      <c r="N230" s="45" t="s">
+      <c r="N230" s="36" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="231" spans="1:14" s="45" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A231" s="45" t="s">
+    <row r="231" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A231" s="36" t="s">
         <v>600</v>
       </c>
-      <c r="B231" s="45" t="s">
-        <v>56</v>
-      </c>
-      <c r="C231" s="45" t="s">
+      <c r="B231" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="C231" s="36" t="s">
         <v>601</v>
       </c>
-      <c r="D231" s="46" t="s">
+      <c r="D231" s="32" t="s">
         <v>569</v>
       </c>
-      <c r="E231" s="47" t="s">
-        <v>779</v>
-      </c>
-      <c r="F231" s="48">
-        <v>45792</v>
-      </c>
-      <c r="G231" s="48">
-        <v>45870</v>
-      </c>
-      <c r="H231" s="45" t="s">
+      <c r="E231" s="33" t="s">
+        <v>351</v>
+      </c>
+      <c r="F231" s="41" t="s">
+        <v>740</v>
+      </c>
+      <c r="G231" s="35">
+        <v>45717</v>
+      </c>
+      <c r="H231" s="36" t="s">
         <v>751</v>
       </c>
-      <c r="I231" s="45" t="b">
-        <v>0</v>
-      </c>
-      <c r="J231" s="45" t="b">
-        <v>1</v>
-      </c>
-      <c r="K231" s="47">
+      <c r="I231" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="J231" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="K231" s="33">
         <v>3</v>
       </c>
-      <c r="L231" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="M231" s="47" t="s">
+      <c r="L231" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="M231" s="33" t="s">
         <v>694</v>
       </c>
-      <c r="N231" s="45" t="s">
+      <c r="N231" s="36" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="232" spans="1:14" s="45" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A232" s="45" t="s">
+    <row r="232" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A232" s="36" t="s">
         <v>602</v>
       </c>
-      <c r="B232" s="45" t="s">
-        <v>56</v>
-      </c>
-      <c r="C232" s="45" t="s">
+      <c r="B232" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="C232" s="36" t="s">
         <v>603</v>
       </c>
-      <c r="D232" s="46" t="s">
+      <c r="D232" s="32" t="s">
         <v>569</v>
       </c>
-      <c r="E232" s="47" t="s">
-        <v>779</v>
-      </c>
-      <c r="F232" s="48">
-        <v>45792</v>
-      </c>
-      <c r="G232" s="48">
-        <v>45870</v>
-      </c>
-      <c r="H232" s="45" t="s">
+      <c r="E232" s="33" t="s">
+        <v>351</v>
+      </c>
+      <c r="F232" s="41" t="s">
+        <v>740</v>
+      </c>
+      <c r="G232" s="35">
+        <v>45717</v>
+      </c>
+      <c r="H232" s="36" t="s">
         <v>751</v>
       </c>
-      <c r="I232" s="45" t="b">
-        <v>0</v>
-      </c>
-      <c r="J232" s="45" t="b">
-        <v>0</v>
-      </c>
-      <c r="K232" s="47">
+      <c r="I232" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="J232" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="K232" s="33">
         <v>3</v>
       </c>
-      <c r="L232" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="M232" s="47" t="s">
+      <c r="L232" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="M232" s="33" t="s">
         <v>693</v>
       </c>
-      <c r="N232" s="45" t="s">
+      <c r="N232" s="36" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="233" spans="1:14" s="45" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A233" s="45" t="s">
+    <row r="233" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A233" s="36" t="s">
         <v>604</v>
       </c>
-      <c r="B233" s="45" t="s">
-        <v>56</v>
-      </c>
-      <c r="C233" s="45" t="s">
+      <c r="B233" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="C233" s="36" t="s">
         <v>605</v>
       </c>
-      <c r="D233" s="46" t="s">
+      <c r="D233" s="32" t="s">
         <v>569</v>
       </c>
-      <c r="E233" s="47" t="s">
-        <v>779</v>
-      </c>
-      <c r="F233" s="48">
-        <v>45792</v>
-      </c>
-      <c r="G233" s="48">
-        <v>45870</v>
-      </c>
-      <c r="H233" s="45" t="s">
+      <c r="E233" s="33" t="s">
+        <v>351</v>
+      </c>
+      <c r="F233" s="41" t="s">
+        <v>740</v>
+      </c>
+      <c r="G233" s="35">
+        <v>45717</v>
+      </c>
+      <c r="H233" s="36" t="s">
         <v>751</v>
       </c>
-      <c r="I233" s="45" t="b">
-        <v>0</v>
-      </c>
-      <c r="J233" s="45" t="b">
-        <v>0</v>
-      </c>
-      <c r="K233" s="47">
+      <c r="I233" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="J233" s="36" t="b">
+        <v>0</v>
+      </c>
+      <c r="K233" s="33">
         <v>3</v>
       </c>
-      <c r="L233" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="M233" s="47" t="s">
+      <c r="L233" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="M233" s="33" t="s">
         <v>694</v>
       </c>
-      <c r="N233" s="45" t="s">
+      <c r="N233" s="36" t="s">
         <v>507</v>
       </c>
     </row>
@@ -12625,25 +12622,25 @@
       </c>
     </row>
     <row r="250" spans="1:14" s="45" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A250" s="49" t="s">
+      <c r="A250" s="48" t="s">
         <v>633</v>
       </c>
-      <c r="B250" s="50" t="s">
-        <v>56</v>
-      </c>
-      <c r="C250" s="51" t="s">
+      <c r="B250" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="C250" s="50" t="s">
         <v>637</v>
       </c>
-      <c r="D250" s="52" t="s">
+      <c r="D250" s="51" t="s">
         <v>631</v>
       </c>
-      <c r="E250" s="47" t="s">
+      <c r="E250" s="46" t="s">
         <v>779</v>
       </c>
-      <c r="F250" s="48">
+      <c r="F250" s="47">
         <v>45792</v>
       </c>
-      <c r="G250" s="48">
+      <c r="G250" s="47">
         <v>45817</v>
       </c>
       <c r="H250" s="45" t="s">
@@ -12655,13 +12652,13 @@
       <c r="J250" s="45" t="b">
         <v>1</v>
       </c>
-      <c r="K250" s="47">
+      <c r="K250" s="46">
         <v>3</v>
       </c>
-      <c r="L250" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="M250" s="47" t="s">
+      <c r="L250" s="46" t="s">
+        <v>111</v>
+      </c>
+      <c r="M250" s="46" t="s">
         <v>693</v>
       </c>
       <c r="N250" s="45" t="s">
@@ -12669,25 +12666,25 @@
       </c>
     </row>
     <row r="251" spans="1:14" s="45" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A251" s="49" t="s">
+      <c r="A251" s="48" t="s">
         <v>634</v>
       </c>
-      <c r="B251" s="50" t="s">
-        <v>56</v>
-      </c>
-      <c r="C251" s="51" t="s">
+      <c r="B251" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="C251" s="50" t="s">
         <v>638</v>
       </c>
-      <c r="D251" s="52" t="s">
+      <c r="D251" s="51" t="s">
         <v>631</v>
       </c>
-      <c r="E251" s="47" t="s">
+      <c r="E251" s="46" t="s">
         <v>779</v>
       </c>
-      <c r="F251" s="48">
+      <c r="F251" s="47">
         <v>45792</v>
       </c>
-      <c r="G251" s="48">
+      <c r="G251" s="47">
         <v>45817</v>
       </c>
       <c r="H251" s="45" t="s">
@@ -12699,13 +12696,13 @@
       <c r="J251" s="45" t="b">
         <v>1</v>
       </c>
-      <c r="K251" s="47">
+      <c r="K251" s="46">
         <v>3</v>
       </c>
-      <c r="L251" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="M251" s="47" t="s">
+      <c r="L251" s="46" t="s">
+        <v>111</v>
+      </c>
+      <c r="M251" s="46" t="s">
         <v>694</v>
       </c>
       <c r="N251" s="45" t="s">
@@ -12713,25 +12710,25 @@
       </c>
     </row>
     <row r="252" spans="1:14" s="45" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A252" s="49" t="s">
+      <c r="A252" s="48" t="s">
         <v>635</v>
       </c>
-      <c r="B252" s="50" t="s">
-        <v>56</v>
-      </c>
-      <c r="C252" s="51" t="s">
+      <c r="B252" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="C252" s="50" t="s">
         <v>639</v>
       </c>
-      <c r="D252" s="52" t="s">
+      <c r="D252" s="51" t="s">
         <v>631</v>
       </c>
-      <c r="E252" s="47" t="s">
+      <c r="E252" s="46" t="s">
         <v>779</v>
       </c>
-      <c r="F252" s="48">
+      <c r="F252" s="47">
         <v>45792</v>
       </c>
-      <c r="G252" s="48">
+      <c r="G252" s="47">
         <v>45817</v>
       </c>
       <c r="H252" s="45" t="s">
@@ -12743,13 +12740,13 @@
       <c r="J252" s="45" t="b">
         <v>1</v>
       </c>
-      <c r="K252" s="47">
+      <c r="K252" s="46">
         <v>3</v>
       </c>
-      <c r="L252" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="M252" s="47" t="s">
+      <c r="L252" s="46" t="s">
+        <v>111</v>
+      </c>
+      <c r="M252" s="46" t="s">
         <v>693</v>
       </c>
       <c r="N252" s="45" t="s">
@@ -12757,25 +12754,25 @@
       </c>
     </row>
     <row r="253" spans="1:14" s="45" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A253" s="49" t="s">
+      <c r="A253" s="48" t="s">
         <v>636</v>
       </c>
-      <c r="B253" s="50" t="s">
-        <v>56</v>
-      </c>
-      <c r="C253" s="51" t="s">
+      <c r="B253" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="C253" s="50" t="s">
         <v>640</v>
       </c>
-      <c r="D253" s="52" t="s">
+      <c r="D253" s="51" t="s">
         <v>631</v>
       </c>
-      <c r="E253" s="47" t="s">
+      <c r="E253" s="46" t="s">
         <v>779</v>
       </c>
-      <c r="F253" s="48">
+      <c r="F253" s="47">
         <v>45792</v>
       </c>
-      <c r="G253" s="48">
+      <c r="G253" s="47">
         <v>45817</v>
       </c>
       <c r="H253" s="45" t="s">
@@ -12787,13 +12784,13 @@
       <c r="J253" s="45" t="b">
         <v>1</v>
       </c>
-      <c r="K253" s="47">
+      <c r="K253" s="46">
         <v>3</v>
       </c>
-      <c r="L253" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="M253" s="47" t="s">
+      <c r="L253" s="46" t="s">
+        <v>111</v>
+      </c>
+      <c r="M253" s="46" t="s">
         <v>694</v>
       </c>
       <c r="N253" s="45" t="s">

</xml_diff>

<commit_message>
Added eB2B document types; TICC-376
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Document types v9.1.xlsx
+++ b/work-in-progress/Peppol Code Lists - Document types v9.1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\peppol-edec-codelists\work-in-progress\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D30077CD-8446-45DE-B11A-455823A18F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FAE16A-BF01-494C-ABDD-CDD48BD87A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17895" yWindow="135" windowWidth="25560" windowHeight="20745" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Document Type" sheetId="5" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2482" uniqueCount="781">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2635" uniqueCount="825">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -2450,6 +2450,145 @@
   <si>
     <t>TICC-328
 TICC-374</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:Invoice-2::Invoice##urn:cen.eu:en16931:2017#conformant#urn:peppol:eb2b:1.0::2.1</t>
+  </si>
+  <si>
+    <t>TICC-376</t>
+  </si>
+  <si>
+    <t>eB2B</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:peppol:eb2b:billing
+cenbii-procid-ubl::urn:peppol:eb2b:order_desadv_billing
+cenbii-procid-ubl::urn:peppol:eb2b:ordering_desadv_billing</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:CreditNote-2::CreditNote##urn:cen.eu:en16931:2017#conformant#urn:peppol:eb2b:1.0::2.1</t>
+  </si>
+  <si>
+    <t>EN 16931 Invoice - eB2B Extension</t>
+  </si>
+  <si>
+    <t>EN 16931 Credit Note - eB2B Extension</t>
+  </si>
+  <si>
+    <t>urn:peppol:doctype:edifact:ORDERS##eb2b::0</t>
+  </si>
+  <si>
+    <t>EDIFACT Order - eB2B Extension</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:peppol:eb2b:order
+cenbii-procid-ubl::urn:peppol:eb2b:ordering
+cenbii-procid-ubl::urn:peppol:eb2b:order_desadv_billing
+cenbii-procid-ubl::urn:peppol:eb2b:ordering_desadv_billing</t>
+  </si>
+  <si>
+    <t>urn:peppol:doctype:edifact:ORDRSP##eb2b::0</t>
+  </si>
+  <si>
+    <t>EDIFACT Order Response - eB2B Extension</t>
+  </si>
+  <si>
+    <t>urn:peppol:doctype:edifact:DESADV##eb2b::0</t>
+  </si>
+  <si>
+    <t>EDIFACT Despatch Advice - eB2B Extension</t>
+  </si>
+  <si>
+    <t>urn:peppol:doctype:edifact:INVOIC##eb2b::0</t>
+  </si>
+  <si>
+    <t>EDIFACT Invoice - eB2B Extension</t>
+  </si>
+  <si>
+    <t>urn:peppol:doctype:x12:850##eb2b::0</t>
+  </si>
+  <si>
+    <t>X12 Order - eB2B Extension</t>
+  </si>
+  <si>
+    <t>X12 Order Response - eB2B Extension</t>
+  </si>
+  <si>
+    <t>X12 Despatch Advice - eB2B Extension</t>
+  </si>
+  <si>
+    <t>X12 Invoice - eB2B Extension</t>
+  </si>
+  <si>
+    <t>urn:peppol:doctype:x12:855##eb2b::0</t>
+  </si>
+  <si>
+    <t>urn:peppol:doctype:x12:856##eb2b::0</t>
+  </si>
+  <si>
+    <t>urn:peppol:doctype:x12:810##eb2b::0</t>
+  </si>
+  <si>
+    <t>Hybrid Order - eB2B Extension</t>
+  </si>
+  <si>
+    <t>urn:peppol:doctype:pdf+xml##eb2b:order-x:1.0::0</t>
+  </si>
+  <si>
+    <t>urn:peppol:doctype:pdf+xml##eb2b:factur-x:1.0::0</t>
+  </si>
+  <si>
+    <t>Hybrid Invoice - eB2B Extension</t>
+  </si>
+  <si>
+    <t>urn:peppol:doctype:bilateral##eb2b:order::0</t>
+  </si>
+  <si>
+    <t>Bilaterally agreed Order - eB2B Extension</t>
+  </si>
+  <si>
+    <t>urn:peppol:doctype:bilateral##eb2b:order_response::0</t>
+  </si>
+  <si>
+    <t>Bilaterally agreed Order Response - eB2B Extension</t>
+  </si>
+  <si>
+    <t>urn:peppol:doctype:bilateral##eb2b:despatch_advice::0</t>
+  </si>
+  <si>
+    <t>Bilaterally agreed Despatch Advice - eB2B Extension</t>
+  </si>
+  <si>
+    <t>urn:peppol:doctype:bilateral##eb2b:invoice::0</t>
+  </si>
+  <si>
+    <t>Bilaterally agreed Invoice - eB2B Extension</t>
+  </si>
+  <si>
+    <t>urn:peppol:doctype:bilateral##eb2b:bilateral::0</t>
+  </si>
+  <si>
+    <t>Bilaterally agreed Document - eB2B Extension</t>
+  </si>
+  <si>
+    <t>Bilateral</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:peppol:eb2b:ordering
+cenbii-procid-ubl::urn:peppol:eb2b:ordering_desadv_billing</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:peppol:eb2b:order_desadv_billing
+cenbii-procid-ubl::urn:peppol:eb2b:ordering_desadv_billing</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:peppol:eb2b:order</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:peppol:eb2b:billing</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:peppol:eb2b:oneway</t>
   </si>
 </sst>
 </file>
@@ -3135,11 +3274,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45987FB-91F4-488D-A9D3-2F3FAED3E07C}">
-  <dimension ref="A1:N283"/>
+  <dimension ref="A1:N300"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A222" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A233" sqref="A233"/>
+      <pane ySplit="1" topLeftCell="A285" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C300" sqref="C300"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13903,6 +14042,618 @@
         <v>507</v>
       </c>
     </row>
+    <row r="284" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A284" s="5" t="s">
+        <v>786</v>
+      </c>
+      <c r="B284" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C284" s="5" t="s">
+        <v>781</v>
+      </c>
+      <c r="D284" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="E284" s="23" t="s">
+        <v>352</v>
+      </c>
+      <c r="H284" s="5" t="s">
+        <v>782</v>
+      </c>
+      <c r="I284" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J284" s="5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="L284" s="23" t="s">
+        <v>783</v>
+      </c>
+      <c r="M284" s="23" t="s">
+        <v>693</v>
+      </c>
+      <c r="N284" s="5" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="285" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A285" s="5" t="s">
+        <v>787</v>
+      </c>
+      <c r="B285" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C285" s="5" t="s">
+        <v>785</v>
+      </c>
+      <c r="D285" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="E285" s="23" t="s">
+        <v>352</v>
+      </c>
+      <c r="H285" s="5" t="s">
+        <v>782</v>
+      </c>
+      <c r="I285" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J285" s="5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="L285" s="23" t="s">
+        <v>783</v>
+      </c>
+      <c r="M285" s="23" t="s">
+        <v>694</v>
+      </c>
+      <c r="N285" s="5" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="286" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A286" s="5" t="s">
+        <v>789</v>
+      </c>
+      <c r="B286" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C286" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="D286" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="E286" s="23" t="s">
+        <v>352</v>
+      </c>
+      <c r="H286" s="5" t="s">
+        <v>782</v>
+      </c>
+      <c r="I286" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J286" s="5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="L286" s="23" t="s">
+        <v>783</v>
+      </c>
+      <c r="M286" s="23" t="s">
+        <v>692</v>
+      </c>
+      <c r="N286" s="5" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="287" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A287" s="5" t="s">
+        <v>792</v>
+      </c>
+      <c r="B287" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C287" s="5" t="s">
+        <v>791</v>
+      </c>
+      <c r="D287" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="E287" s="23" t="s">
+        <v>352</v>
+      </c>
+      <c r="H287" s="5" t="s">
+        <v>782</v>
+      </c>
+      <c r="I287" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J287" s="5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="L287" s="23" t="s">
+        <v>783</v>
+      </c>
+      <c r="M287" s="23" t="s">
+        <v>695</v>
+      </c>
+      <c r="N287" s="5" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="288" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A288" s="5" t="s">
+        <v>794</v>
+      </c>
+      <c r="B288" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C288" s="5" t="s">
+        <v>793</v>
+      </c>
+      <c r="D288" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="E288" s="23" t="s">
+        <v>352</v>
+      </c>
+      <c r="H288" s="5" t="s">
+        <v>782</v>
+      </c>
+      <c r="I288" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J288" s="5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="L288" s="23" t="s">
+        <v>783</v>
+      </c>
+      <c r="M288" s="23" t="s">
+        <v>696</v>
+      </c>
+      <c r="N288" s="5" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="289" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A289" s="5" t="s">
+        <v>796</v>
+      </c>
+      <c r="B289" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C289" s="5" t="s">
+        <v>795</v>
+      </c>
+      <c r="D289" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="E289" s="23" t="s">
+        <v>352</v>
+      </c>
+      <c r="H289" s="5" t="s">
+        <v>782</v>
+      </c>
+      <c r="I289" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J289" s="5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="L289" s="23" t="s">
+        <v>783</v>
+      </c>
+      <c r="M289" s="23" t="s">
+        <v>693</v>
+      </c>
+      <c r="N289" s="5" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="290" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A290" s="5" t="s">
+        <v>798</v>
+      </c>
+      <c r="B290" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C290" s="5" t="s">
+        <v>797</v>
+      </c>
+      <c r="D290" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="E290" s="23" t="s">
+        <v>352</v>
+      </c>
+      <c r="H290" s="5" t="s">
+        <v>782</v>
+      </c>
+      <c r="I290" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J290" s="5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="L290" s="23" t="s">
+        <v>783</v>
+      </c>
+      <c r="M290" s="23" t="s">
+        <v>692</v>
+      </c>
+      <c r="N290" s="5" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="291" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A291" s="5" t="s">
+        <v>799</v>
+      </c>
+      <c r="B291" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C291" s="5" t="s">
+        <v>802</v>
+      </c>
+      <c r="D291" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="E291" s="23" t="s">
+        <v>352</v>
+      </c>
+      <c r="H291" s="5" t="s">
+        <v>782</v>
+      </c>
+      <c r="I291" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J291" s="5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="L291" s="23" t="s">
+        <v>783</v>
+      </c>
+      <c r="M291" s="23" t="s">
+        <v>695</v>
+      </c>
+      <c r="N291" s="5" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="292" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A292" s="5" t="s">
+        <v>800</v>
+      </c>
+      <c r="B292" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C292" s="5" t="s">
+        <v>803</v>
+      </c>
+      <c r="D292" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="E292" s="23" t="s">
+        <v>352</v>
+      </c>
+      <c r="H292" s="5" t="s">
+        <v>782</v>
+      </c>
+      <c r="I292" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J292" s="5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="L292" s="23" t="s">
+        <v>783</v>
+      </c>
+      <c r="M292" s="23" t="s">
+        <v>696</v>
+      </c>
+      <c r="N292" s="5" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="293" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A293" s="5" t="s">
+        <v>801</v>
+      </c>
+      <c r="B293" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C293" s="5" t="s">
+        <v>804</v>
+      </c>
+      <c r="D293" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="E293" s="23" t="s">
+        <v>352</v>
+      </c>
+      <c r="H293" s="5" t="s">
+        <v>782</v>
+      </c>
+      <c r="I293" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J293" s="5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="L293" s="23" t="s">
+        <v>783</v>
+      </c>
+      <c r="M293" s="23" t="s">
+        <v>693</v>
+      </c>
+      <c r="N293" s="5" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="294" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A294" s="5" t="s">
+        <v>805</v>
+      </c>
+      <c r="B294" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C294" s="5" t="s">
+        <v>806</v>
+      </c>
+      <c r="D294" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="E294" s="23" t="s">
+        <v>352</v>
+      </c>
+      <c r="H294" s="5" t="s">
+        <v>782</v>
+      </c>
+      <c r="I294" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J294" s="5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="L294" s="23" t="s">
+        <v>783</v>
+      </c>
+      <c r="M294" s="23" t="s">
+        <v>692</v>
+      </c>
+      <c r="N294" s="5" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="295" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A295" s="5" t="s">
+        <v>808</v>
+      </c>
+      <c r="B295" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C295" s="5" t="s">
+        <v>807</v>
+      </c>
+      <c r="D295" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="E295" s="23" t="s">
+        <v>352</v>
+      </c>
+      <c r="H295" s="5" t="s">
+        <v>782</v>
+      </c>
+      <c r="I295" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J295" s="5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="L295" s="23" t="s">
+        <v>783</v>
+      </c>
+      <c r="M295" s="23" t="s">
+        <v>693</v>
+      </c>
+      <c r="N295" s="5" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="296" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A296" s="5" t="s">
+        <v>810</v>
+      </c>
+      <c r="B296" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C296" s="5" t="s">
+        <v>809</v>
+      </c>
+      <c r="D296" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="E296" s="23" t="s">
+        <v>352</v>
+      </c>
+      <c r="H296" s="5" t="s">
+        <v>782</v>
+      </c>
+      <c r="I296" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J296" s="5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="L296" s="23" t="s">
+        <v>783</v>
+      </c>
+      <c r="M296" s="23" t="s">
+        <v>692</v>
+      </c>
+      <c r="N296" s="5" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="297" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A297" s="5" t="s">
+        <v>812</v>
+      </c>
+      <c r="B297" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C297" s="5" t="s">
+        <v>811</v>
+      </c>
+      <c r="D297" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="E297" s="23" t="s">
+        <v>352</v>
+      </c>
+      <c r="H297" s="5" t="s">
+        <v>782</v>
+      </c>
+      <c r="I297" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J297" s="5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="L297" s="23" t="s">
+        <v>783</v>
+      </c>
+      <c r="M297" s="23" t="s">
+        <v>695</v>
+      </c>
+      <c r="N297" s="5" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="298" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A298" s="5" t="s">
+        <v>814</v>
+      </c>
+      <c r="B298" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C298" s="5" t="s">
+        <v>813</v>
+      </c>
+      <c r="D298" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="E298" s="23" t="s">
+        <v>352</v>
+      </c>
+      <c r="H298" s="5" t="s">
+        <v>782</v>
+      </c>
+      <c r="I298" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J298" s="5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="L298" s="23" t="s">
+        <v>783</v>
+      </c>
+      <c r="M298" s="23" t="s">
+        <v>696</v>
+      </c>
+      <c r="N298" s="5" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="299" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A299" s="5" t="s">
+        <v>816</v>
+      </c>
+      <c r="B299" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C299" s="5" t="s">
+        <v>815</v>
+      </c>
+      <c r="D299" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="E299" s="23" t="s">
+        <v>352</v>
+      </c>
+      <c r="H299" s="5" t="s">
+        <v>782</v>
+      </c>
+      <c r="I299" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J299" s="5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="L299" s="23" t="s">
+        <v>783</v>
+      </c>
+      <c r="M299" s="23" t="s">
+        <v>693</v>
+      </c>
+      <c r="N299" s="5" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="300" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A300" s="5" t="s">
+        <v>818</v>
+      </c>
+      <c r="B300" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C300" s="5" t="s">
+        <v>817</v>
+      </c>
+      <c r="D300" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="E300" s="23" t="s">
+        <v>352</v>
+      </c>
+      <c r="H300" s="5" t="s">
+        <v>782</v>
+      </c>
+      <c r="I300" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J300" s="5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="L300" s="23" t="s">
+        <v>783</v>
+      </c>
+      <c r="M300" s="23" t="s">
+        <v>819</v>
+      </c>
+      <c r="N300" s="5" t="s">
+        <v>824</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:N283" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Marked old Reporting DocTypes as removed
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Document types v9.1.xlsx
+++ b/work-in-progress/Peppol Code Lists - Document types v9.1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\edec-codelists\work-in-progress\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\peppol-edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FAE16A-BF01-494C-ABDD-CDD48BD87A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB2CB0D2-0851-420D-8DE3-B6696B9C844D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25410" yWindow="135" windowWidth="25560" windowHeight="20745" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Document Type" sheetId="5" r:id="rId1"/>
@@ -3277,8 +3277,8 @@
   <dimension ref="A1:N300"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A285" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C300" sqref="C300"/>
+      <pane ySplit="1" topLeftCell="A171" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A182" sqref="A182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10131,83 +10131,87 @@
         <v>123</v>
       </c>
     </row>
-    <row r="181" spans="1:14" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A181" s="36" t="s">
+    <row r="181" spans="1:14" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A181" s="44" t="s">
         <v>459</v>
       </c>
-      <c r="B181" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="C181" s="36" t="s">
+      <c r="B181" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C181" s="15" t="s">
         <v>424</v>
       </c>
-      <c r="D181" s="37" t="s">
+      <c r="D181" s="29" t="s">
         <v>415</v>
       </c>
-      <c r="E181" s="33" t="s">
-        <v>351</v>
-      </c>
-      <c r="F181" s="40" t="s">
+      <c r="E181" s="24" t="s">
+        <v>482</v>
+      </c>
+      <c r="F181" s="21" t="s">
         <v>569</v>
       </c>
-      <c r="G181" s="35"/>
-      <c r="H181" s="36" t="s">
+      <c r="G181" s="18">
+        <v>45658</v>
+      </c>
+      <c r="H181" s="15" t="s">
         <v>587</v>
       </c>
-      <c r="I181" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="J181" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="K181" s="33"/>
-      <c r="L181" s="33" t="s">
+      <c r="I181" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J181" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="K181" s="24"/>
+      <c r="L181" s="24" t="s">
         <v>426</v>
       </c>
-      <c r="M181" s="33" t="s">
+      <c r="M181" s="24" t="s">
         <v>706</v>
       </c>
-      <c r="N181" s="36" t="s">
+      <c r="N181" s="19" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="182" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A182" s="36" t="s">
+    <row r="182" spans="1:14" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A182" s="44" t="s">
         <v>460</v>
       </c>
-      <c r="B182" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="C182" s="36" t="s">
+      <c r="B182" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C182" s="15" t="s">
         <v>427</v>
       </c>
-      <c r="D182" s="37" t="s">
+      <c r="D182" s="29" t="s">
         <v>415</v>
       </c>
-      <c r="E182" s="33" t="s">
-        <v>351</v>
-      </c>
-      <c r="F182" s="40" t="s">
+      <c r="E182" s="24" t="s">
+        <v>482</v>
+      </c>
+      <c r="F182" s="21" t="s">
         <v>569</v>
       </c>
-      <c r="G182" s="35"/>
-      <c r="H182" s="36" t="s">
+      <c r="G182" s="18">
+        <v>45658</v>
+      </c>
+      <c r="H182" s="15" t="s">
         <v>587</v>
       </c>
-      <c r="I182" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="J182" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="K182" s="33"/>
-      <c r="L182" s="33" t="s">
+      <c r="I182" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J182" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="K182" s="24"/>
+      <c r="L182" s="24" t="s">
         <v>426</v>
       </c>
-      <c r="M182" s="33" t="s">
+      <c r="M182" s="24" t="s">
         <v>706</v>
       </c>
-      <c r="N182" s="36" t="s">
+      <c r="N182" s="19" t="s">
         <v>425</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added AE TDD and TDS identifiers; TICC-373
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Document types v9.1.xlsx
+++ b/work-in-progress/Peppol Code Lists - Document types v9.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\peppol-edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD39644A-3164-4154-A3AD-0DF64D70D75F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AFE215C-6C38-414E-81BC-A5E9EE634F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25410" yWindow="135" windowWidth="25560" windowHeight="20745" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2635" uniqueCount="825">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2653" uniqueCount="831">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -2589,6 +2589,24 @@
   </si>
   <si>
     <t>cenbii-procid-ubl::urn:peppol:eb2b:oneway</t>
+  </si>
+  <si>
+    <t>urn:fdc:peppol:tax-data-document:1.0::TaxData##urn:peppol:pint:taxdata-1@ae-1::1.0</t>
+  </si>
+  <si>
+    <t>urn:fdc:peppol:tax-data-status:1.0::TaxDataStatus##urn:peppol:pint:taxdatastatus-1@ae-1::1.0</t>
+  </si>
+  <si>
+    <t>Tax Reporting</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:peppol:bis:taxreporting</t>
+  </si>
+  <si>
+    <t>AE Tax Data Document v1.0</t>
+  </si>
+  <si>
+    <t>AE Tax Data Status v1.0</t>
   </si>
 </sst>
 </file>
@@ -3274,11 +3292,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45987FB-91F4-488D-A9D3-2F3FAED3E07C}">
-  <dimension ref="A1:N300"/>
+  <dimension ref="A1:N302"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A171" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G182" sqref="G182"/>
+      <pane ySplit="1" topLeftCell="A276" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A286" sqref="A286"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14046,15 +14064,15 @@
         <v>507</v>
       </c>
     </row>
-    <row r="284" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A284" s="5" t="s">
-        <v>786</v>
+    <row r="284" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>829</v>
       </c>
       <c r="B284" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C284" s="5" t="s">
-        <v>781</v>
+        <v>588</v>
+      </c>
+      <c r="C284" s="1" t="s">
+        <v>825</v>
       </c>
       <c r="D284" s="28" t="s">
         <v>740</v>
@@ -14063,7 +14081,7 @@
         <v>352</v>
       </c>
       <c r="H284" s="5" t="s">
-        <v>782</v>
+        <v>750</v>
       </c>
       <c r="I284" s="5" t="b">
         <v>0</v>
@@ -14073,24 +14091,24 @@
         <v>1</v>
       </c>
       <c r="L284" s="23" t="s">
-        <v>783</v>
+        <v>111</v>
       </c>
       <c r="M284" s="23" t="s">
-        <v>693</v>
+        <v>827</v>
       </c>
       <c r="N284" s="5" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="285" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A285" s="5" t="s">
-        <v>787</v>
+        <v>828</v>
+      </c>
+    </row>
+    <row r="285" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>830</v>
       </c>
       <c r="B285" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C285" s="5" t="s">
-        <v>785</v>
+        <v>588</v>
+      </c>
+      <c r="C285" s="1" t="s">
+        <v>826</v>
       </c>
       <c r="D285" s="28" t="s">
         <v>740</v>
@@ -14099,7 +14117,7 @@
         <v>352</v>
       </c>
       <c r="H285" s="5" t="s">
-        <v>782</v>
+        <v>750</v>
       </c>
       <c r="I285" s="5" t="b">
         <v>0</v>
@@ -14109,24 +14127,24 @@
         <v>1</v>
       </c>
       <c r="L285" s="23" t="s">
-        <v>783</v>
+        <v>111</v>
       </c>
       <c r="M285" s="23" t="s">
-        <v>694</v>
+        <v>827</v>
       </c>
       <c r="N285" s="5" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="286" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="286" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A286" s="5" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="B286" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C286" s="5" t="s">
-        <v>788</v>
+        <v>781</v>
       </c>
       <c r="D286" s="28" t="s">
         <v>740</v>
@@ -14148,21 +14166,21 @@
         <v>783</v>
       </c>
       <c r="M286" s="23" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="N286" s="5" t="s">
-        <v>790</v>
-      </c>
-    </row>
-    <row r="287" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="287" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A287" s="5" t="s">
-        <v>792</v>
+        <v>787</v>
       </c>
       <c r="B287" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C287" s="5" t="s">
-        <v>791</v>
+        <v>785</v>
       </c>
       <c r="D287" s="28" t="s">
         <v>740</v>
@@ -14184,21 +14202,21 @@
         <v>783</v>
       </c>
       <c r="M287" s="23" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="N287" s="5" t="s">
-        <v>820</v>
-      </c>
-    </row>
-    <row r="288" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="288" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A288" s="5" t="s">
-        <v>794</v>
+        <v>789</v>
       </c>
       <c r="B288" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C288" s="5" t="s">
-        <v>793</v>
+        <v>788</v>
       </c>
       <c r="D288" s="28" t="s">
         <v>740</v>
@@ -14220,21 +14238,21 @@
         <v>783</v>
       </c>
       <c r="M288" s="23" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="N288" s="5" t="s">
-        <v>821</v>
-      </c>
-    </row>
-    <row r="289" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="289" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A289" s="5" t="s">
-        <v>796</v>
+        <v>792</v>
       </c>
       <c r="B289" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C289" s="5" t="s">
-        <v>795</v>
+        <v>791</v>
       </c>
       <c r="D289" s="28" t="s">
         <v>740</v>
@@ -14256,21 +14274,21 @@
         <v>783</v>
       </c>
       <c r="M289" s="23" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="N289" s="5" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="290" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="290" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A290" s="5" t="s">
-        <v>798</v>
+        <v>794</v>
       </c>
       <c r="B290" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C290" s="5" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
       <c r="D290" s="28" t="s">
         <v>740</v>
@@ -14292,21 +14310,21 @@
         <v>783</v>
       </c>
       <c r="M290" s="23" t="s">
-        <v>692</v>
+        <v>696</v>
       </c>
       <c r="N290" s="5" t="s">
-        <v>790</v>
-      </c>
-    </row>
-    <row r="291" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="291" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A291" s="5" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
       <c r="B291" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C291" s="5" t="s">
-        <v>802</v>
+        <v>795</v>
       </c>
       <c r="D291" s="28" t="s">
         <v>740</v>
@@ -14328,21 +14346,21 @@
         <v>783</v>
       </c>
       <c r="M291" s="23" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="N291" s="5" t="s">
-        <v>820</v>
-      </c>
-    </row>
-    <row r="292" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="292" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A292" s="5" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="B292" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C292" s="5" t="s">
-        <v>803</v>
+        <v>797</v>
       </c>
       <c r="D292" s="28" t="s">
         <v>740</v>
@@ -14364,21 +14382,21 @@
         <v>783</v>
       </c>
       <c r="M292" s="23" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="N292" s="5" t="s">
-        <v>821</v>
-      </c>
-    </row>
-    <row r="293" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="293" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A293" s="5" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="B293" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C293" s="5" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="D293" s="28" t="s">
         <v>740</v>
@@ -14400,21 +14418,21 @@
         <v>783</v>
       </c>
       <c r="M293" s="23" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="N293" s="5" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="294" spans="1:14" x14ac:dyDescent="0.25">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="294" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A294" s="5" t="s">
-        <v>805</v>
+        <v>800</v>
       </c>
       <c r="B294" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C294" s="5" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="D294" s="28" t="s">
         <v>740</v>
@@ -14436,21 +14454,21 @@
         <v>783</v>
       </c>
       <c r="M294" s="23" t="s">
-        <v>692</v>
+        <v>696</v>
       </c>
       <c r="N294" s="5" t="s">
-        <v>822</v>
-      </c>
-    </row>
-    <row r="295" spans="1:14" x14ac:dyDescent="0.25">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="295" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A295" s="5" t="s">
-        <v>808</v>
+        <v>801</v>
       </c>
       <c r="B295" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C295" s="5" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
       <c r="D295" s="28" t="s">
         <v>740</v>
@@ -14475,18 +14493,18 @@
         <v>693</v>
       </c>
       <c r="N295" s="5" t="s">
-        <v>823</v>
-      </c>
-    </row>
-    <row r="296" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="296" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A296" s="5" t="s">
-        <v>810</v>
+        <v>805</v>
       </c>
       <c r="B296" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C296" s="5" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
       <c r="D296" s="28" t="s">
         <v>740</v>
@@ -14511,18 +14529,18 @@
         <v>692</v>
       </c>
       <c r="N296" s="5" t="s">
-        <v>790</v>
-      </c>
-    </row>
-    <row r="297" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="297" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A297" s="5" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="B297" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C297" s="5" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="D297" s="28" t="s">
         <v>740</v>
@@ -14544,21 +14562,21 @@
         <v>783</v>
       </c>
       <c r="M297" s="23" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="N297" s="5" t="s">
-        <v>820</v>
-      </c>
-    </row>
-    <row r="298" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="298" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A298" s="5" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="B298" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C298" s="5" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="D298" s="28" t="s">
         <v>740</v>
@@ -14580,21 +14598,21 @@
         <v>783</v>
       </c>
       <c r="M298" s="23" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="N298" s="5" t="s">
-        <v>821</v>
-      </c>
-    </row>
-    <row r="299" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="299" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A299" s="5" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="B299" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C299" s="5" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
       <c r="D299" s="28" t="s">
         <v>740</v>
@@ -14616,21 +14634,21 @@
         <v>783</v>
       </c>
       <c r="M299" s="23" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="N299" s="5" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="300" spans="1:14" x14ac:dyDescent="0.25">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="300" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A300" s="5" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
       <c r="B300" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C300" s="5" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="D300" s="28" t="s">
         <v>740</v>
@@ -14652,9 +14670,81 @@
         <v>783</v>
       </c>
       <c r="M300" s="23" t="s">
+        <v>696</v>
+      </c>
+      <c r="N300" s="5" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="301" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A301" s="5" t="s">
+        <v>816</v>
+      </c>
+      <c r="B301" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C301" s="5" t="s">
+        <v>815</v>
+      </c>
+      <c r="D301" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="E301" s="23" t="s">
+        <v>352</v>
+      </c>
+      <c r="H301" s="5" t="s">
+        <v>782</v>
+      </c>
+      <c r="I301" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J301" s="5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="L301" s="23" t="s">
+        <v>783</v>
+      </c>
+      <c r="M301" s="23" t="s">
+        <v>693</v>
+      </c>
+      <c r="N301" s="5" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="302" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A302" s="5" t="s">
+        <v>818</v>
+      </c>
+      <c r="B302" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C302" s="5" t="s">
+        <v>817</v>
+      </c>
+      <c r="D302" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="E302" s="23" t="s">
+        <v>352</v>
+      </c>
+      <c r="H302" s="5" t="s">
+        <v>782</v>
+      </c>
+      <c r="I302" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J302" s="5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="L302" s="23" t="s">
+        <v>783</v>
+      </c>
+      <c r="M302" s="23" t="s">
         <v>819</v>
       </c>
-      <c r="N300" s="5" t="s">
+      <c r="N302" s="5" t="s">
         <v>824</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added DICO Maintenance Status; TICC-360
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Document types v9.1.xlsx
+++ b/work-in-progress/Peppol Code Lists - Document types v9.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\peppol-edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AFE215C-6C38-414E-81BC-A5E9EE634F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39BE87DE-0293-4139-BDC9-0560BB0DE064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25410" yWindow="135" windowWidth="25560" windowHeight="20745" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2653" uniqueCount="831">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2662" uniqueCount="834">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -2607,6 +2607,15 @@
   </si>
   <si>
     <t>AE Tax Data Status v1.0</t>
+  </si>
+  <si>
+    <t>DICO Maintenance Status</t>
+  </si>
+  <si>
+    <t>http://www.ketenstandaard.nl/onderhoudsstatus/SALES/005::MaintenanceStatus##dico:maintenancestatus@nl-1.0::1.0</t>
+  </si>
+  <si>
+    <t>TICC-360</t>
   </si>
 </sst>
 </file>
@@ -3292,11 +3301,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45987FB-91F4-488D-A9D3-2F3FAED3E07C}">
-  <dimension ref="A1:N302"/>
+  <dimension ref="A1:N303"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A276" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A286" sqref="A286"/>
+      <pane ySplit="1" topLeftCell="A292" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A304" sqref="A304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14748,6 +14757,41 @@
         <v>824</v>
       </c>
     </row>
+    <row r="303" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A303" s="5" t="s">
+        <v>831</v>
+      </c>
+      <c r="B303" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C303" s="5" t="s">
+        <v>832</v>
+      </c>
+      <c r="D303" s="28" t="s">
+        <v>740</v>
+      </c>
+      <c r="E303" s="23" t="s">
+        <v>352</v>
+      </c>
+      <c r="H303" s="5" t="s">
+        <v>833</v>
+      </c>
+      <c r="I303" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J303" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="L303" s="23" t="s">
+        <v>580</v>
+      </c>
+      <c r="M303" s="23" t="s">
+        <v>716</v>
+      </c>
+      <c r="N303" s="5" t="s">
+        <v>713</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:N283" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>